<commit_message>
Added Excel to Hashmap logic to Anikas Framework
</commit_message>
<xml_diff>
--- a/src/test/resources/testData/Driver.xlsx
+++ b/src/test/resources/testData/Driver.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="591" uniqueCount="212">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="650" uniqueCount="246">
   <si>
     <t>Parameteres</t>
   </si>
@@ -427,16 +427,10 @@
     <t>MCC2100-CSP6</t>
   </si>
   <si>
-    <t>ProMS</t>
-  </si>
-  <si>
     <t>UAT</t>
   </si>
   <si>
     <t>NewOpp1</t>
-  </si>
-  <si>
-    <t>8.6</t>
   </si>
   <si>
     <t>5/19/2020</t>
@@ -663,13 +657,121 @@
   </si>
   <si>
     <t>http://www.newtours.demoaut.com</t>
+  </si>
+  <si>
+    <t>WebTours</t>
+  </si>
+  <si>
+    <t>rautsumit2</t>
+  </si>
+  <si>
+    <t>myCase2</t>
+  </si>
+  <si>
+    <t>team</t>
+  </si>
+  <si>
+    <t>role</t>
+  </si>
+  <si>
+    <t>anika</t>
+  </si>
+  <si>
+    <t>ketki</t>
+  </si>
+  <si>
+    <t>sumt</t>
+  </si>
+  <si>
+    <t>CEO</t>
+  </si>
+  <si>
+    <t>CTO</t>
+  </si>
+  <si>
+    <t>Common man</t>
+  </si>
+  <si>
+    <t>salary</t>
+  </si>
+  <si>
+    <t>1000000</t>
+  </si>
+  <si>
+    <t>1500000</t>
+  </si>
+  <si>
+    <t>10000</t>
+  </si>
+  <si>
+    <t>type</t>
+  </si>
+  <si>
+    <t>passengers</t>
+  </si>
+  <si>
+    <t>departing_from</t>
+  </si>
+  <si>
+    <t>arriving_in</t>
+  </si>
+  <si>
+    <t>returning_month</t>
+  </si>
+  <si>
+    <t>returning_day</t>
+  </si>
+  <si>
+    <t>preferences</t>
+  </si>
+  <si>
+    <t>airline</t>
+  </si>
+  <si>
+    <t>2</t>
+  </si>
+  <si>
+    <t>London</t>
+  </si>
+  <si>
+    <t xml:space="preserve">New yok </t>
+  </si>
+  <si>
+    <t>June</t>
+  </si>
+  <si>
+    <t>Business class</t>
+  </si>
+  <si>
+    <t>Unified Airlines</t>
+  </si>
+  <si>
+    <t>departing_month</t>
+  </si>
+  <si>
+    <t>departing_day</t>
+  </si>
+  <si>
+    <t>WT_Register</t>
+  </si>
+  <si>
+    <t>na</t>
+  </si>
+  <si>
+    <t>3</t>
+  </si>
+  <si>
+    <t>6</t>
+  </si>
+  <si>
+    <t>yes</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="10" x14ac:knownFonts="1">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -734,6 +836,12 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="10">
@@ -1036,7 +1144,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="108">
+  <cellXfs count="125">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -1302,12 +1410,52 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="49" fontId="4" fillId="3" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="3" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="4" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="3" fillId="4" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="4" borderId="8" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="4" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="4" borderId="8" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="4" fillId="4" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="49" fontId="9" fillId="4" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="4" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="4" borderId="8" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="49" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="3" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
@@ -1315,6 +1463,9 @@
       <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="3" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="3" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1709,16 +1860,16 @@
       <c r="B1" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="C1" s="104" t="s">
+      <c r="C1" s="120" t="s">
         <v>0</v>
       </c>
-      <c r="D1" s="104"/>
-      <c r="E1" s="104"/>
-      <c r="F1" s="104"/>
-      <c r="G1" s="104"/>
-      <c r="H1" s="104"/>
-      <c r="I1" s="104"/>
-      <c r="J1" s="104"/>
+      <c r="D1" s="120"/>
+      <c r="E1" s="120"/>
+      <c r="F1" s="120"/>
+      <c r="G1" s="120"/>
+      <c r="H1" s="120"/>
+      <c r="I1" s="120"/>
+      <c r="J1" s="120"/>
     </row>
     <row r="2" spans="1:23" s="4" customFormat="1" ht="45" x14ac:dyDescent="0.3">
       <c r="A2" s="24">
@@ -1901,7 +2052,7 @@
         <v>7</v>
       </c>
       <c r="D6" s="16" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="E6" s="26" t="s">
         <v>30</v>
@@ -2097,10 +2248,10 @@
         <v>128</v>
       </c>
       <c r="N10" s="85" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="O10" s="85" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="P10" s="26" t="s">
         <v>133</v>
@@ -2135,7 +2286,7 @@
         <v>7</v>
       </c>
       <c r="D12" s="66" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="E12" s="66" t="s">
         <v>125</v>
@@ -2147,10 +2298,10 @@
         <v>62</v>
       </c>
       <c r="H12" s="86" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="I12" s="68" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="J12" s="68" t="s">
         <v>66</v>
@@ -2159,19 +2310,19 @@
         <v>130</v>
       </c>
       <c r="L12" s="69" t="s">
+        <v>143</v>
+      </c>
+      <c r="M12" s="66" t="s">
+        <v>144</v>
+      </c>
+      <c r="N12" s="66" t="s">
+        <v>168</v>
+      </c>
+      <c r="O12" s="66" t="s">
+        <v>136</v>
+      </c>
+      <c r="P12" s="66" t="s">
         <v>145</v>
-      </c>
-      <c r="M12" s="66" t="s">
-        <v>146</v>
-      </c>
-      <c r="N12" s="66" t="s">
-        <v>170</v>
-      </c>
-      <c r="O12" s="66" t="s">
-        <v>138</v>
-      </c>
-      <c r="P12" s="66" t="s">
-        <v>147</v>
       </c>
       <c r="Q12" s="66">
         <v>1</v>
@@ -2203,46 +2354,46 @@
         <v>7</v>
       </c>
       <c r="D14" s="66" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="E14" s="26" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="F14" s="26" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="G14" s="76" t="s">
         <v>62</v>
       </c>
       <c r="H14" s="87" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="I14" s="68" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="J14" s="68" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="K14" s="66" t="s">
         <v>130</v>
       </c>
       <c r="L14" s="69" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="M14" s="66" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="N14" s="26" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="O14" s="26" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="P14" s="66" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="Q14" s="26" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
     </row>
     <row r="15" spans="1:23" s="11" customFormat="1" x14ac:dyDescent="0.25">
@@ -2271,46 +2422,46 @@
         <v>7</v>
       </c>
       <c r="D16" s="66" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="E16" s="26" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="F16" s="26" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="G16" s="17" t="s">
         <v>62</v>
       </c>
       <c r="H16" s="87" t="s">
+        <v>150</v>
+      </c>
+      <c r="I16" s="80" t="s">
+        <v>151</v>
+      </c>
+      <c r="J16" s="14" t="s">
         <v>152</v>
-      </c>
-      <c r="I16" s="80" t="s">
-        <v>153</v>
-      </c>
-      <c r="J16" s="14" t="s">
-        <v>154</v>
       </c>
       <c r="K16" s="66" t="s">
         <v>130</v>
       </c>
       <c r="L16" s="69" t="s">
+        <v>153</v>
+      </c>
+      <c r="M16" s="26" t="s">
+        <v>154</v>
+      </c>
+      <c r="N16" s="26" t="s">
+        <v>173</v>
+      </c>
+      <c r="O16" s="26" t="s">
+        <v>168</v>
+      </c>
+      <c r="P16" s="26" t="s">
         <v>155</v>
       </c>
-      <c r="M16" s="26" t="s">
-        <v>156</v>
-      </c>
-      <c r="N16" s="26" t="s">
-        <v>175</v>
-      </c>
-      <c r="O16" s="26" t="s">
-        <v>170</v>
-      </c>
-      <c r="P16" s="26" t="s">
-        <v>157</v>
-      </c>
       <c r="Q16" s="26" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
     </row>
     <row r="17" spans="1:17" s="11" customFormat="1" x14ac:dyDescent="0.25">
@@ -2339,46 +2490,46 @@
         <v>7</v>
       </c>
       <c r="D18" s="66" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="E18" s="26" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="F18" s="26" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="G18" s="17" t="s">
         <v>62</v>
       </c>
       <c r="H18" s="87" t="s">
+        <v>162</v>
+      </c>
+      <c r="I18" s="80" t="s">
+        <v>163</v>
+      </c>
+      <c r="J18" s="14" t="s">
         <v>164</v>
-      </c>
-      <c r="I18" s="80" t="s">
-        <v>165</v>
-      </c>
-      <c r="J18" s="14" t="s">
-        <v>166</v>
       </c>
       <c r="K18" s="66" t="s">
         <v>130</v>
       </c>
       <c r="L18" s="69" t="s">
+        <v>165</v>
+      </c>
+      <c r="M18" s="26" t="s">
+        <v>166</v>
+      </c>
+      <c r="N18" s="26" t="s">
+        <v>174</v>
+      </c>
+      <c r="O18" s="26" t="s">
+        <v>172</v>
+      </c>
+      <c r="P18" s="26" t="s">
         <v>167</v>
       </c>
-      <c r="M18" s="26" t="s">
-        <v>168</v>
-      </c>
-      <c r="N18" s="26" t="s">
-        <v>176</v>
-      </c>
-      <c r="O18" s="26" t="s">
-        <v>174</v>
-      </c>
-      <c r="P18" s="26" t="s">
-        <v>169</v>
-      </c>
       <c r="Q18" s="26" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
     </row>
     <row r="19" spans="1:17" s="11" customFormat="1" x14ac:dyDescent="0.25">
@@ -2405,16 +2556,16 @@
         <v>3</v>
       </c>
       <c r="B20" s="12" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="C20" s="16" t="s">
         <v>12</v>
       </c>
       <c r="D20" s="66" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="E20" s="26" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="F20" s="26"/>
       <c r="G20" s="17"/>
@@ -2436,10 +2587,10 @@
         <v>6</v>
       </c>
       <c r="D21" s="26" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="E21" s="26" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="F21" s="26"/>
       <c r="G21" s="17"/>
@@ -2518,16 +2669,16 @@
       <c r="B1" s="36" t="s">
         <v>9</v>
       </c>
-      <c r="C1" s="105" t="s">
+      <c r="C1" s="121" t="s">
         <v>0</v>
       </c>
-      <c r="D1" s="106"/>
-      <c r="E1" s="106"/>
-      <c r="F1" s="106"/>
-      <c r="G1" s="106"/>
-      <c r="H1" s="106"/>
-      <c r="I1" s="106"/>
-      <c r="J1" s="107"/>
+      <c r="D1" s="122"/>
+      <c r="E1" s="122"/>
+      <c r="F1" s="122"/>
+      <c r="G1" s="122"/>
+      <c r="H1" s="122"/>
+      <c r="I1" s="122"/>
+      <c r="J1" s="123"/>
     </row>
     <row r="2" spans="1:21" s="37" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A2" s="38">
@@ -2601,7 +2752,7 @@
         <v>30</v>
       </c>
       <c r="F3" s="45" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="G3" s="45" t="s">
         <v>95</v>
@@ -3664,7 +3815,7 @@
         <v>87</v>
       </c>
       <c r="R29" s="54" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="S29" s="52" t="s">
         <v>75</v>
@@ -3706,7 +3857,7 @@
         <v>11</v>
       </c>
       <c r="B31" s="50" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="C31" s="39" t="s">
         <v>12</v>
@@ -3754,25 +3905,25 @@
         <v>132</v>
       </c>
       <c r="R31" s="50" t="s">
+        <v>187</v>
+      </c>
+      <c r="S31" s="50" t="s">
+        <v>188</v>
+      </c>
+      <c r="T31" s="50" t="s">
         <v>189</v>
       </c>
-      <c r="S31" s="50" t="s">
-        <v>190</v>
-      </c>
-      <c r="T31" s="50" t="s">
-        <v>191</v>
-      </c>
       <c r="U31" s="50" t="s">
+        <v>196</v>
+      </c>
+      <c r="V31" s="50" t="s">
+        <v>197</v>
+      </c>
+      <c r="W31" s="50" t="s">
         <v>198</v>
       </c>
-      <c r="V31" s="50" t="s">
-        <v>199</v>
-      </c>
-      <c r="W31" s="50" t="s">
-        <v>200</v>
-      </c>
       <c r="X31" s="39" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
     </row>
     <row r="32" spans="1:24" s="60" customFormat="1" ht="60" x14ac:dyDescent="0.25">
@@ -3782,7 +3933,7 @@
         <v>7</v>
       </c>
       <c r="D32" s="66" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="E32" s="66" t="s">
         <v>125</v>
@@ -3794,10 +3945,10 @@
         <v>62</v>
       </c>
       <c r="H32" s="95" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="I32" s="94" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="J32" s="68" t="s">
         <v>66</v>
@@ -3806,7 +3957,7 @@
         <v>130</v>
       </c>
       <c r="L32" s="69" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="M32" s="66" t="s">
         <v>128</v>
@@ -3818,31 +3969,31 @@
         <v>62</v>
       </c>
       <c r="P32" s="97" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="Q32" s="97">
         <v>1</v>
       </c>
       <c r="R32" s="97" t="s">
+        <v>175</v>
+      </c>
+      <c r="S32" s="97" t="s">
+        <v>176</v>
+      </c>
+      <c r="T32" s="97" t="s">
         <v>177</v>
       </c>
-      <c r="S32" s="97" t="s">
+      <c r="U32" s="97" t="s">
         <v>178</v>
-      </c>
-      <c r="T32" s="97" t="s">
-        <v>179</v>
-      </c>
-      <c r="U32" s="97" t="s">
-        <v>180</v>
       </c>
       <c r="V32" s="97">
         <v>2000</v>
       </c>
       <c r="W32" s="97" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="X32" s="59" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
     </row>
     <row r="33" spans="1:27" s="92" customFormat="1" x14ac:dyDescent="0.25">
@@ -3878,7 +4029,7 @@
         <v>7</v>
       </c>
       <c r="D34" s="66" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="E34" s="66" t="s">
         <v>125</v>
@@ -3890,7 +4041,7 @@
         <v>62</v>
       </c>
       <c r="H34" s="95" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="I34" s="94" t="s">
         <v>127</v>
@@ -3902,10 +4053,10 @@
         <v>130</v>
       </c>
       <c r="L34" s="69" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="M34" s="66" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="N34" s="66" t="s">
         <v>62</v>
@@ -3914,31 +4065,31 @@
         <v>62</v>
       </c>
       <c r="P34" s="97" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="Q34" s="97">
         <v>1</v>
       </c>
       <c r="R34" s="97" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="S34" s="97">
         <v>1750000</v>
       </c>
       <c r="T34" s="97" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="U34" s="97" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="V34" s="97">
         <v>250000</v>
       </c>
       <c r="W34" s="97" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="X34" s="59" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
     </row>
     <row r="35" spans="1:27" s="92" customFormat="1" x14ac:dyDescent="0.25">
@@ -3974,46 +4125,46 @@
         <v>7</v>
       </c>
       <c r="D36" s="43" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="E36" s="96" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="F36" s="66" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="G36" s="90" t="s">
         <v>62</v>
       </c>
       <c r="H36" s="90" t="s">
+        <v>181</v>
+      </c>
+      <c r="I36" s="90" t="s">
+        <v>142</v>
+      </c>
+      <c r="J36" s="90" t="s">
+        <v>182</v>
+      </c>
+      <c r="K36" s="90" t="s">
         <v>183</v>
       </c>
-      <c r="I36" s="90" t="s">
-        <v>144</v>
-      </c>
-      <c r="J36" s="90" t="s">
-        <v>184</v>
-      </c>
-      <c r="K36" s="90" t="s">
-        <v>185</v>
-      </c>
       <c r="L36" s="90" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="M36" s="90" t="s">
         <v>128</v>
       </c>
       <c r="N36" s="90" t="s">
+        <v>184</v>
+      </c>
+      <c r="O36" s="90" t="s">
+        <v>185</v>
+      </c>
+      <c r="P36" s="97" t="s">
         <v>186</v>
       </c>
-      <c r="O36" s="90" t="s">
-        <v>187</v>
-      </c>
-      <c r="P36" s="97" t="s">
-        <v>188</v>
-      </c>
       <c r="Q36" s="97" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="R36" s="97" t="s">
         <v>62</v>
@@ -4034,7 +4185,7 @@
         <v>62</v>
       </c>
       <c r="X36" s="61" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="Y36" s="61"/>
     </row>
@@ -4055,10 +4206,10 @@
       <c r="N37" s="96"/>
       <c r="O37" s="96"/>
       <c r="P37" s="97" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="Q37" s="97" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="R37" s="97" t="s">
         <v>62</v>
@@ -4079,7 +4230,7 @@
         <v>62</v>
       </c>
       <c r="X37" s="61" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
     </row>
     <row r="38" spans="1:27" s="37" customFormat="1" ht="30" x14ac:dyDescent="0.25">
@@ -4099,31 +4250,31 @@
       <c r="N38" s="96"/>
       <c r="O38" s="96"/>
       <c r="P38" s="97" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="Q38" s="97" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="R38" s="97" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="S38" s="101">
         <v>100000</v>
       </c>
       <c r="T38" s="97" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="U38" s="97" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="V38" s="101">
         <v>25000</v>
       </c>
       <c r="W38" s="97" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="X38" s="61" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
     </row>
     <row r="39" spans="1:27" s="37" customFormat="1" ht="30" x14ac:dyDescent="0.25">
@@ -4143,31 +4294,31 @@
       <c r="N39" s="96"/>
       <c r="O39" s="96"/>
       <c r="P39" s="97" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="Q39" s="97" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="R39" s="97" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="S39" s="101">
         <v>200000</v>
       </c>
       <c r="T39" s="97" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="U39" s="97" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="V39" s="101">
         <v>50000</v>
       </c>
       <c r="W39" s="97" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="X39" s="61" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
     </row>
     <row r="40" spans="1:27" s="37" customFormat="1" x14ac:dyDescent="0.25">
@@ -4187,10 +4338,10 @@
       <c r="N40" s="96"/>
       <c r="O40" s="96"/>
       <c r="P40" s="97" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="Q40" s="97" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="R40" s="97" t="s">
         <v>62</v>
@@ -4231,31 +4382,31 @@
       <c r="N41" s="96"/>
       <c r="O41" s="96"/>
       <c r="P41" s="97" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="Q41" s="97" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="R41" s="97" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="S41" s="101">
         <v>1300370</v>
       </c>
       <c r="T41" s="97" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="U41" s="97" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="V41" s="101">
         <v>237740</v>
       </c>
       <c r="W41" s="97" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="X41" s="61" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
     </row>
     <row r="42" spans="1:27" s="37" customFormat="1" x14ac:dyDescent="0.25">
@@ -4291,46 +4442,46 @@
         <v>7</v>
       </c>
       <c r="D43" s="43" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="E43" s="96" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="F43" s="66" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="G43" s="90" t="s">
         <v>62</v>
       </c>
       <c r="H43" s="90" t="s">
+        <v>181</v>
+      </c>
+      <c r="I43" s="90" t="s">
+        <v>142</v>
+      </c>
+      <c r="J43" s="90" t="s">
+        <v>182</v>
+      </c>
+      <c r="K43" s="90" t="s">
         <v>183</v>
       </c>
-      <c r="I43" s="90" t="s">
-        <v>144</v>
-      </c>
-      <c r="J43" s="90" t="s">
-        <v>184</v>
-      </c>
-      <c r="K43" s="90" t="s">
-        <v>185</v>
-      </c>
       <c r="L43" s="90" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="M43" s="90" t="s">
         <v>128</v>
       </c>
       <c r="N43" s="90" t="s">
+        <v>184</v>
+      </c>
+      <c r="O43" s="90" t="s">
+        <v>185</v>
+      </c>
+      <c r="P43" s="97" t="s">
         <v>186</v>
       </c>
-      <c r="O43" s="90" t="s">
-        <v>187</v>
-      </c>
-      <c r="P43" s="97" t="s">
-        <v>188</v>
-      </c>
       <c r="Q43" s="97" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="R43" s="97" t="s">
         <v>62</v>
@@ -4351,7 +4502,7 @@
         <v>62</v>
       </c>
       <c r="X43" s="61" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
     </row>
     <row r="44" spans="1:27" s="37" customFormat="1" x14ac:dyDescent="0.25">
@@ -4442,7 +4593,7 @@
         <v>3</v>
       </c>
       <c r="B1" s="25" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="C1" s="25" t="s">
         <v>17</v>
@@ -4462,7 +4613,7 @@
         <v>13</v>
       </c>
       <c r="B2" s="102" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="C2" s="20" t="s">
         <v>18</v>
@@ -4482,7 +4633,7 @@
         <v>14</v>
       </c>
       <c r="B3" s="102" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="C3" s="20" t="s">
         <v>18</v>
@@ -4499,10 +4650,10 @@
     </row>
     <row r="4" spans="1:6" ht="30.75" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A4" s="18" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B4" s="102" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="C4" s="20" t="s">
         <v>18</v>
@@ -4546,7 +4697,7 @@
   <dimension ref="A1:B7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.3"/>
@@ -4574,7 +4725,7 @@
         <v>5</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>134</v>
+        <v>210</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
@@ -4582,7 +4733,7 @@
         <v>3</v>
       </c>
       <c r="B3" s="13" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="15.75" x14ac:dyDescent="0.3">
@@ -4603,8 +4754,8 @@
       <c r="A6" s="21" t="s">
         <v>16</v>
       </c>
-      <c r="B6" s="2" t="s">
-        <v>137</v>
+      <c r="B6" s="2">
+        <v>0</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.3">
@@ -4634,176 +4785,622 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:W6"/>
+  <dimension ref="A1:W20"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="84" zoomScaleNormal="84" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6:XFD6"/>
+      <selection activeCell="C1" sqref="C1:J1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="6" width="9.140625" style="119"/>
+    <col min="7" max="7" width="10.7109375" style="119" bestFit="1" customWidth="1"/>
+    <col min="8" max="13" width="9.140625" style="119"/>
+    <col min="14" max="14" width="16.42578125" style="119" bestFit="1" customWidth="1"/>
+    <col min="15" max="16384" width="9.140625" style="119"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:23" s="103" customFormat="1" ht="90" x14ac:dyDescent="0.3">
-      <c r="A1" s="8" t="s">
+    <row r="1" spans="1:23" s="104" customFormat="1" ht="90" x14ac:dyDescent="0.3">
+      <c r="A1" s="103" t="s">
         <v>4</v>
       </c>
-      <c r="B1" s="8" t="s">
+      <c r="B1" s="103" t="s">
         <v>9</v>
       </c>
-      <c r="C1" s="104" t="s">
+      <c r="C1" s="124" t="s">
         <v>0</v>
       </c>
-      <c r="D1" s="104"/>
-      <c r="E1" s="104"/>
-      <c r="F1" s="104"/>
-      <c r="G1" s="104"/>
-      <c r="H1" s="104"/>
-      <c r="I1" s="104"/>
-      <c r="J1" s="104"/>
-    </row>
-    <row r="2" spans="1:23" s="4" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="24">
+      <c r="D1" s="124"/>
+      <c r="E1" s="124"/>
+      <c r="F1" s="124"/>
+      <c r="G1" s="124"/>
+      <c r="H1" s="124"/>
+      <c r="I1" s="124"/>
+      <c r="J1" s="124"/>
+    </row>
+    <row r="2" spans="1:23" s="108" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="105">
         <v>1</v>
       </c>
-      <c r="B2" s="24" t="s">
+      <c r="B2" s="105" t="s">
+        <v>204</v>
+      </c>
+      <c r="C2" s="106" t="s">
+        <v>12</v>
+      </c>
+      <c r="D2" s="106" t="s">
+        <v>205</v>
+      </c>
+      <c r="E2" s="106" t="s">
         <v>206</v>
       </c>
-      <c r="C2" s="15" t="s">
+      <c r="F2" s="106"/>
+      <c r="G2" s="106"/>
+      <c r="H2" s="106"/>
+      <c r="I2" s="106"/>
+      <c r="J2" s="106"/>
+      <c r="K2" s="106"/>
+      <c r="L2" s="106"/>
+      <c r="M2" s="106"/>
+      <c r="N2" s="106"/>
+      <c r="O2" s="106"/>
+      <c r="P2" s="106"/>
+      <c r="Q2" s="106"/>
+      <c r="R2" s="106"/>
+      <c r="S2" s="106"/>
+      <c r="T2" s="106"/>
+      <c r="U2" s="106"/>
+      <c r="V2" s="107"/>
+      <c r="W2" s="107"/>
+    </row>
+    <row r="3" spans="1:23" s="108" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A3" s="109"/>
+      <c r="B3" s="110"/>
+      <c r="C3" s="111" t="s">
+        <v>245</v>
+      </c>
+      <c r="D3" s="111" t="s">
+        <v>208</v>
+      </c>
+      <c r="E3" s="96" t="s">
+        <v>208</v>
+      </c>
+      <c r="F3" s="96"/>
+      <c r="G3" s="96"/>
+      <c r="H3" s="96"/>
+      <c r="I3" s="96"/>
+      <c r="J3" s="96"/>
+      <c r="K3" s="96"/>
+      <c r="L3" s="96"/>
+      <c r="M3" s="112"/>
+      <c r="N3" s="112"/>
+      <c r="O3" s="96"/>
+      <c r="P3" s="96"/>
+      <c r="Q3" s="96"/>
+      <c r="R3" s="96"/>
+      <c r="S3" s="106"/>
+      <c r="T3" s="113"/>
+      <c r="U3" s="106"/>
+      <c r="V3" s="107"/>
+      <c r="W3" s="107"/>
+    </row>
+    <row r="4" spans="1:23" s="106" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="114"/>
+      <c r="B4" s="110"/>
+      <c r="C4" s="111"/>
+      <c r="D4" s="96"/>
+      <c r="E4" s="96"/>
+      <c r="F4" s="96"/>
+      <c r="G4" s="112"/>
+      <c r="H4" s="115"/>
+      <c r="I4" s="116"/>
+      <c r="J4" s="116"/>
+      <c r="K4" s="96"/>
+      <c r="L4" s="117"/>
+      <c r="M4" s="96"/>
+      <c r="N4" s="96"/>
+      <c r="O4" s="96"/>
+      <c r="P4" s="96"/>
+      <c r="Q4" s="96"/>
+    </row>
+    <row r="5" spans="1:23" s="108" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A5" s="109"/>
+      <c r="B5" s="110"/>
+      <c r="C5" s="111" t="s">
+        <v>245</v>
+      </c>
+      <c r="D5" s="111" t="s">
+        <v>211</v>
+      </c>
+      <c r="E5" s="96" t="s">
+        <v>208</v>
+      </c>
+      <c r="F5" s="96"/>
+      <c r="G5" s="96"/>
+      <c r="H5" s="96"/>
+      <c r="I5" s="96"/>
+      <c r="J5" s="96"/>
+      <c r="K5" s="96"/>
+      <c r="L5" s="96"/>
+      <c r="M5" s="112"/>
+      <c r="N5" s="112"/>
+      <c r="O5" s="96"/>
+      <c r="P5" s="96"/>
+      <c r="Q5" s="96"/>
+      <c r="R5" s="96"/>
+      <c r="S5" s="106"/>
+      <c r="T5" s="113"/>
+      <c r="U5" s="106"/>
+      <c r="V5" s="107"/>
+      <c r="W5" s="107"/>
+    </row>
+    <row r="6" spans="1:23" s="106" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="114"/>
+      <c r="B6" s="110"/>
+      <c r="C6" s="111"/>
+      <c r="D6" s="96"/>
+      <c r="E6" s="96"/>
+      <c r="F6" s="96"/>
+      <c r="G6" s="112"/>
+      <c r="H6" s="115"/>
+      <c r="I6" s="116"/>
+      <c r="J6" s="116"/>
+      <c r="K6" s="96"/>
+      <c r="L6" s="117"/>
+      <c r="M6" s="96"/>
+      <c r="N6" s="96"/>
+      <c r="O6" s="96"/>
+      <c r="P6" s="96"/>
+      <c r="Q6" s="96"/>
+    </row>
+    <row r="7" spans="1:23" s="108" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A7" s="109"/>
+      <c r="B7" s="110"/>
+      <c r="C7" s="111" t="s">
+        <v>245</v>
+      </c>
+      <c r="D7" s="111" t="s">
+        <v>208</v>
+      </c>
+      <c r="E7" s="96" t="s">
+        <v>208</v>
+      </c>
+      <c r="F7" s="96"/>
+      <c r="G7" s="96"/>
+      <c r="H7" s="96"/>
+      <c r="I7" s="96"/>
+      <c r="J7" s="96"/>
+      <c r="K7" s="96"/>
+      <c r="L7" s="96"/>
+      <c r="M7" s="112"/>
+      <c r="N7" s="112"/>
+      <c r="O7" s="96"/>
+      <c r="P7" s="96"/>
+      <c r="Q7" s="96"/>
+      <c r="R7" s="96"/>
+      <c r="S7" s="106"/>
+      <c r="T7" s="113"/>
+      <c r="U7" s="106"/>
+      <c r="V7" s="107"/>
+      <c r="W7" s="107"/>
+    </row>
+    <row r="8" spans="1:23" s="106" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="114"/>
+      <c r="B8" s="110"/>
+      <c r="C8" s="111"/>
+      <c r="D8" s="96"/>
+      <c r="E8" s="96"/>
+      <c r="F8" s="96"/>
+      <c r="G8" s="112"/>
+      <c r="H8" s="115"/>
+      <c r="I8" s="116"/>
+      <c r="J8" s="116"/>
+      <c r="K8" s="96"/>
+      <c r="L8" s="117"/>
+      <c r="M8" s="96"/>
+      <c r="N8" s="96"/>
+      <c r="O8" s="96"/>
+      <c r="P8" s="96"/>
+      <c r="Q8" s="96"/>
+    </row>
+    <row r="9" spans="1:23" s="108" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="105">
+        <v>2</v>
+      </c>
+      <c r="B9" s="105" t="s">
+        <v>212</v>
+      </c>
+      <c r="C9" s="106" t="s">
         <v>12</v>
       </c>
-      <c r="D2" s="15" t="s">
-        <v>207</v>
-      </c>
-      <c r="E2" s="15" t="s">
+      <c r="D9" s="106" t="s">
+        <v>213</v>
+      </c>
+      <c r="E9" s="106" t="s">
+        <v>214</v>
+      </c>
+      <c r="F9" s="106" t="s">
+        <v>221</v>
+      </c>
+      <c r="G9" s="106"/>
+      <c r="H9" s="106"/>
+      <c r="I9" s="106"/>
+      <c r="J9" s="106"/>
+      <c r="K9" s="106"/>
+      <c r="L9" s="106"/>
+      <c r="M9" s="106"/>
+      <c r="N9" s="106"/>
+      <c r="O9" s="106"/>
+      <c r="P9" s="106"/>
+      <c r="Q9" s="106"/>
+      <c r="R9" s="106"/>
+      <c r="S9" s="106"/>
+      <c r="T9" s="106"/>
+      <c r="U9" s="106"/>
+      <c r="V9" s="107"/>
+      <c r="W9" s="107"/>
+    </row>
+    <row r="10" spans="1:23" s="108" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="109"/>
+      <c r="B10" s="110"/>
+      <c r="C10" s="111" t="s">
+        <v>245</v>
+      </c>
+      <c r="D10" s="111" t="s">
+        <v>215</v>
+      </c>
+      <c r="E10" s="96" t="s">
+        <v>218</v>
+      </c>
+      <c r="F10" s="96" t="s">
+        <v>222</v>
+      </c>
+      <c r="G10" s="96"/>
+      <c r="H10" s="96"/>
+      <c r="I10" s="96"/>
+      <c r="J10" s="96"/>
+      <c r="K10" s="96"/>
+      <c r="L10" s="96"/>
+      <c r="M10" s="112"/>
+      <c r="N10" s="112"/>
+      <c r="O10" s="96"/>
+      <c r="P10" s="96"/>
+      <c r="Q10" s="96"/>
+      <c r="R10" s="96"/>
+      <c r="S10" s="106"/>
+      <c r="T10" s="113"/>
+      <c r="U10" s="106"/>
+      <c r="V10" s="107"/>
+      <c r="W10" s="107"/>
+    </row>
+    <row r="11" spans="1:23" s="106" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="114"/>
+      <c r="B11" s="110"/>
+      <c r="C11" s="111"/>
+      <c r="D11" s="96"/>
+      <c r="E11" s="96"/>
+      <c r="F11" s="96"/>
+      <c r="G11" s="112"/>
+      <c r="H11" s="115"/>
+      <c r="I11" s="116"/>
+      <c r="J11" s="116"/>
+      <c r="K11" s="96"/>
+      <c r="L11" s="117"/>
+      <c r="M11" s="96"/>
+      <c r="N11" s="96"/>
+      <c r="O11" s="96"/>
+      <c r="P11" s="96"/>
+      <c r="Q11" s="96"/>
+    </row>
+    <row r="12" spans="1:23" s="108" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="109"/>
+      <c r="B12" s="110"/>
+      <c r="C12" s="111" t="s">
+        <v>245</v>
+      </c>
+      <c r="D12" s="111" t="s">
+        <v>216</v>
+      </c>
+      <c r="E12" s="96" t="s">
+        <v>219</v>
+      </c>
+      <c r="F12" s="96" t="s">
+        <v>223</v>
+      </c>
+      <c r="G12" s="96"/>
+      <c r="H12" s="96"/>
+      <c r="I12" s="96"/>
+      <c r="J12" s="96"/>
+      <c r="K12" s="96"/>
+      <c r="L12" s="96"/>
+      <c r="M12" s="112"/>
+      <c r="N12" s="112"/>
+      <c r="O12" s="96"/>
+      <c r="P12" s="96"/>
+      <c r="Q12" s="96"/>
+      <c r="R12" s="96"/>
+      <c r="S12" s="106"/>
+      <c r="T12" s="113"/>
+      <c r="U12" s="106"/>
+      <c r="V12" s="107"/>
+      <c r="W12" s="107"/>
+    </row>
+    <row r="13" spans="1:23" s="106" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="114"/>
+      <c r="B13" s="110"/>
+      <c r="C13" s="111"/>
+      <c r="D13" s="96"/>
+      <c r="E13" s="96"/>
+      <c r="F13" s="96"/>
+      <c r="G13" s="112"/>
+      <c r="H13" s="115"/>
+      <c r="I13" s="116"/>
+      <c r="J13" s="116"/>
+      <c r="K13" s="96"/>
+      <c r="L13" s="117"/>
+      <c r="M13" s="96"/>
+      <c r="N13" s="96"/>
+      <c r="O13" s="96"/>
+      <c r="P13" s="96"/>
+      <c r="Q13" s="96"/>
+    </row>
+    <row r="14" spans="1:23" s="108" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A14" s="109"/>
+      <c r="B14" s="110"/>
+      <c r="C14" s="111" t="s">
+        <v>245</v>
+      </c>
+      <c r="D14" s="111" t="s">
+        <v>217</v>
+      </c>
+      <c r="E14" s="96" t="s">
+        <v>220</v>
+      </c>
+      <c r="F14" s="96" t="s">
+        <v>224</v>
+      </c>
+      <c r="G14" s="96"/>
+      <c r="H14" s="96"/>
+      <c r="I14" s="96"/>
+      <c r="J14" s="96"/>
+      <c r="K14" s="96"/>
+      <c r="L14" s="96"/>
+      <c r="M14" s="112"/>
+      <c r="N14" s="112"/>
+      <c r="O14" s="96"/>
+      <c r="P14" s="96"/>
+      <c r="Q14" s="96"/>
+      <c r="R14" s="96"/>
+      <c r="S14" s="106"/>
+      <c r="T14" s="113"/>
+      <c r="U14" s="106"/>
+      <c r="V14" s="107"/>
+      <c r="W14" s="107"/>
+    </row>
+    <row r="15" spans="1:23" s="106" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="114"/>
+      <c r="B15" s="110"/>
+      <c r="C15" s="111"/>
+      <c r="D15" s="96"/>
+      <c r="E15" s="96"/>
+      <c r="F15" s="96"/>
+      <c r="G15" s="112"/>
+      <c r="H15" s="115"/>
+      <c r="I15" s="116"/>
+      <c r="J15" s="116"/>
+      <c r="K15" s="96"/>
+      <c r="L15" s="117"/>
+      <c r="M15" s="96"/>
+      <c r="N15" s="96"/>
+      <c r="O15" s="96"/>
+      <c r="P15" s="96"/>
+      <c r="Q15" s="96"/>
+    </row>
+    <row r="16" spans="1:23" s="108" customFormat="1" ht="30" x14ac:dyDescent="0.3">
+      <c r="A16" s="105">
+        <v>3</v>
+      </c>
+      <c r="B16" s="105" t="s">
+        <v>241</v>
+      </c>
+      <c r="C16" s="106" t="s">
+        <v>12</v>
+      </c>
+      <c r="D16" s="106" t="s">
+        <v>205</v>
+      </c>
+      <c r="E16" s="106" t="s">
+        <v>206</v>
+      </c>
+      <c r="F16" s="106" t="s">
+        <v>225</v>
+      </c>
+      <c r="G16" s="106" t="s">
+        <v>226</v>
+      </c>
+      <c r="H16" s="106" t="s">
+        <v>227</v>
+      </c>
+      <c r="I16" s="106" t="s">
+        <v>239</v>
+      </c>
+      <c r="J16" s="106" t="s">
+        <v>240</v>
+      </c>
+      <c r="K16" s="106" t="s">
+        <v>228</v>
+      </c>
+      <c r="L16" s="106" t="s">
+        <v>229</v>
+      </c>
+      <c r="M16" s="106" t="s">
+        <v>230</v>
+      </c>
+      <c r="N16" s="106" t="s">
+        <v>231</v>
+      </c>
+      <c r="O16" s="106" t="s">
+        <v>232</v>
+      </c>
+      <c r="P16" s="106"/>
+      <c r="Q16" s="106"/>
+      <c r="R16" s="106"/>
+      <c r="S16" s="106"/>
+      <c r="T16" s="106"/>
+      <c r="U16" s="106"/>
+      <c r="V16" s="107"/>
+      <c r="W16" s="107"/>
+    </row>
+    <row r="17" spans="1:23" s="108" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A17" s="109"/>
+      <c r="B17" s="110"/>
+      <c r="C17" s="111" t="s">
+        <v>6</v>
+      </c>
+      <c r="D17" s="111" t="s">
         <v>208</v>
       </c>
-      <c r="F2" s="15"/>
-      <c r="G2" s="15"/>
-      <c r="H2" s="15"/>
-      <c r="I2" s="15"/>
-      <c r="J2" s="15"/>
-      <c r="K2" s="15"/>
-      <c r="L2" s="15"/>
-      <c r="M2" s="15"/>
-      <c r="N2" s="15"/>
-      <c r="O2" s="15"/>
-      <c r="P2" s="11"/>
-      <c r="Q2" s="11"/>
-      <c r="R2" s="11"/>
-      <c r="S2" s="11"/>
-      <c r="T2" s="11"/>
-      <c r="U2" s="11"/>
-      <c r="V2" s="5"/>
-      <c r="W2" s="5"/>
-    </row>
-    <row r="3" spans="1:23" s="4" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A3" s="9"/>
-      <c r="B3" s="12"/>
-      <c r="C3" s="16" t="s">
+      <c r="E17" s="96" t="s">
+        <v>208</v>
+      </c>
+      <c r="F17" s="96" t="s">
+        <v>242</v>
+      </c>
+      <c r="G17" s="96" t="s">
+        <v>233</v>
+      </c>
+      <c r="H17" s="96" t="s">
+        <v>234</v>
+      </c>
+      <c r="I17" s="96" t="s">
+        <v>236</v>
+      </c>
+      <c r="J17" s="96" t="s">
+        <v>146</v>
+      </c>
+      <c r="K17" s="96" t="s">
+        <v>235</v>
+      </c>
+      <c r="L17" s="96" t="s">
+        <v>244</v>
+      </c>
+      <c r="M17" s="96" t="s">
+        <v>243</v>
+      </c>
+      <c r="N17" s="118" t="s">
+        <v>237</v>
+      </c>
+      <c r="O17" s="96" t="s">
+        <v>238</v>
+      </c>
+      <c r="P17" s="96"/>
+      <c r="Q17" s="96"/>
+      <c r="R17" s="96"/>
+      <c r="S17" s="106"/>
+      <c r="T17" s="113"/>
+      <c r="U17" s="106"/>
+      <c r="V17" s="107"/>
+      <c r="W17" s="107"/>
+    </row>
+    <row r="18" spans="1:23" s="106" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="114"/>
+      <c r="B18" s="110"/>
+      <c r="C18" s="111"/>
+      <c r="D18" s="96"/>
+      <c r="E18" s="96"/>
+      <c r="F18" s="96"/>
+      <c r="G18" s="112"/>
+      <c r="H18" s="115"/>
+      <c r="I18" s="116"/>
+      <c r="J18" s="116"/>
+      <c r="K18" s="96"/>
+      <c r="L18" s="117"/>
+      <c r="M18" s="96"/>
+      <c r="N18" s="96"/>
+      <c r="O18" s="96"/>
+      <c r="P18" s="96"/>
+      <c r="Q18" s="96"/>
+    </row>
+    <row r="19" spans="1:23" s="108" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A19" s="109"/>
+      <c r="B19" s="110"/>
+      <c r="C19" s="111" t="s">
         <v>6</v>
       </c>
-      <c r="D3" s="16" t="s">
-        <v>210</v>
-      </c>
-      <c r="E3" s="26" t="s">
-        <v>210</v>
-      </c>
-      <c r="F3" s="26"/>
-      <c r="G3" s="26"/>
-      <c r="H3" s="26"/>
-      <c r="I3" s="26"/>
-      <c r="J3" s="26"/>
-      <c r="K3" s="26"/>
-      <c r="L3" s="26"/>
-      <c r="M3" s="17"/>
-      <c r="N3" s="17"/>
-      <c r="O3" s="26"/>
-      <c r="P3" s="26"/>
-      <c r="Q3" s="26"/>
-      <c r="R3" s="26"/>
-      <c r="S3" s="11"/>
-      <c r="T3"/>
-      <c r="U3" s="11"/>
-      <c r="V3" s="5"/>
-      <c r="W3" s="5"/>
-    </row>
-    <row r="4" spans="1:23" s="70" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="63"/>
-      <c r="B4" s="64"/>
-      <c r="C4" s="71"/>
-      <c r="D4" s="26"/>
-      <c r="E4" s="26"/>
-      <c r="F4" s="73"/>
-      <c r="G4" s="75"/>
-      <c r="H4" s="87"/>
-      <c r="I4" s="14"/>
-      <c r="J4" s="68"/>
-      <c r="K4" s="66"/>
-      <c r="L4" s="69"/>
-      <c r="M4" s="66"/>
-      <c r="N4" s="66"/>
-      <c r="O4" s="66"/>
-      <c r="P4" s="66"/>
-      <c r="Q4" s="66"/>
-    </row>
-    <row r="5" spans="1:23" s="4" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A5" s="9"/>
-      <c r="B5" s="12"/>
-      <c r="C5" s="16" t="s">
-        <v>6</v>
-      </c>
-      <c r="D5" s="16" t="s">
-        <v>210</v>
-      </c>
-      <c r="E5" s="26" t="s">
-        <v>210</v>
-      </c>
-      <c r="F5" s="26"/>
-      <c r="G5" s="26"/>
-      <c r="H5" s="26"/>
-      <c r="I5" s="26"/>
-      <c r="J5" s="26"/>
-      <c r="K5" s="26"/>
-      <c r="L5" s="26"/>
-      <c r="M5" s="17"/>
-      <c r="N5" s="17"/>
-      <c r="O5" s="26"/>
-      <c r="P5" s="26"/>
-      <c r="Q5" s="26"/>
-      <c r="R5" s="26"/>
-      <c r="S5" s="11"/>
-      <c r="T5"/>
-      <c r="U5" s="11"/>
-      <c r="V5" s="5"/>
-      <c r="W5" s="5"/>
-    </row>
-    <row r="6" spans="1:23" s="70" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="63"/>
-      <c r="B6" s="64"/>
-      <c r="C6" s="71"/>
-      <c r="D6" s="26"/>
-      <c r="E6" s="26"/>
-      <c r="F6" s="73"/>
-      <c r="G6" s="75"/>
-      <c r="H6" s="87"/>
-      <c r="I6" s="14"/>
-      <c r="J6" s="68"/>
-      <c r="K6" s="66"/>
-      <c r="L6" s="69"/>
-      <c r="M6" s="66"/>
-      <c r="N6" s="66"/>
-      <c r="O6" s="66"/>
-      <c r="P6" s="66"/>
-      <c r="Q6" s="66"/>
+      <c r="D19" s="111" t="s">
+        <v>208</v>
+      </c>
+      <c r="E19" s="96" t="s">
+        <v>208</v>
+      </c>
+      <c r="F19" s="96" t="s">
+        <v>242</v>
+      </c>
+      <c r="G19" s="96" t="s">
+        <v>243</v>
+      </c>
+      <c r="H19" s="96" t="s">
+        <v>234</v>
+      </c>
+      <c r="I19" s="96" t="s">
+        <v>236</v>
+      </c>
+      <c r="J19" s="96" t="s">
+        <v>146</v>
+      </c>
+      <c r="K19" s="96" t="s">
+        <v>235</v>
+      </c>
+      <c r="L19" s="96" t="s">
+        <v>244</v>
+      </c>
+      <c r="M19" s="96" t="s">
+        <v>243</v>
+      </c>
+      <c r="N19" s="118" t="s">
+        <v>237</v>
+      </c>
+      <c r="O19" s="96" t="s">
+        <v>238</v>
+      </c>
+      <c r="P19" s="96"/>
+      <c r="Q19" s="96"/>
+      <c r="R19" s="96"/>
+      <c r="S19" s="106"/>
+      <c r="T19" s="113"/>
+      <c r="U19" s="106"/>
+      <c r="V19" s="107"/>
+      <c r="W19" s="107"/>
+    </row>
+    <row r="20" spans="1:23" s="106" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="114"/>
+      <c r="B20" s="110"/>
+      <c r="C20" s="111"/>
+      <c r="D20" s="96"/>
+      <c r="E20" s="96"/>
+      <c r="F20" s="96"/>
+      <c r="G20" s="112"/>
+      <c r="H20" s="115"/>
+      <c r="I20" s="116"/>
+      <c r="J20" s="116"/>
+      <c r="K20" s="96"/>
+      <c r="L20" s="117"/>
+      <c r="M20" s="96"/>
+      <c r="N20" s="96"/>
+      <c r="O20" s="96"/>
+      <c r="P20" s="96"/>
+      <c r="Q20" s="96"/>
     </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="C1:J1"/>
   </mergeCells>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" sqref="L1:L6">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" sqref="L1:L16 L18 L20">
       <formula1>"5000,,7000,,8000"</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Adding New Branch for Extent changes
</commit_message>
<xml_diff>
--- a/src/test/resources/testData/Driver.xlsx
+++ b/src/test/resources/testData/Driver.xlsx
@@ -689,9 +689,6 @@
     <t>CTO</t>
   </si>
   <si>
-    <t>Common man</t>
-  </si>
-  <si>
     <t>salary</t>
   </si>
   <si>
@@ -765,6 +762,9 @@
   </si>
   <si>
     <t>yes</t>
+  </si>
+  <si>
+    <t>se</t>
   </si>
 </sst>
 </file>
@@ -4788,7 +4788,7 @@
   <dimension ref="A1:W20"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="84" zoomScaleNormal="84" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1:J1"/>
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4857,7 +4857,7 @@
       <c r="A3" s="109"/>
       <c r="B3" s="110"/>
       <c r="C3" s="111" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="D3" s="111" t="s">
         <v>208</v>
@@ -4907,7 +4907,7 @@
       <c r="A5" s="109"/>
       <c r="B5" s="110"/>
       <c r="C5" s="111" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="D5" s="111" t="s">
         <v>211</v>
@@ -4957,7 +4957,7 @@
       <c r="A7" s="109"/>
       <c r="B7" s="110"/>
       <c r="C7" s="111" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="D7" s="111" t="s">
         <v>208</v>
@@ -5020,7 +5020,7 @@
         <v>214</v>
       </c>
       <c r="F9" s="106" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="G9" s="106"/>
       <c r="H9" s="106"/>
@@ -5044,7 +5044,7 @@
       <c r="A10" s="109"/>
       <c r="B10" s="110"/>
       <c r="C10" s="111" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="D10" s="111" t="s">
         <v>215</v>
@@ -5053,7 +5053,7 @@
         <v>218</v>
       </c>
       <c r="F10" s="96" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="G10" s="96"/>
       <c r="H10" s="96"/>
@@ -5096,7 +5096,7 @@
       <c r="A12" s="109"/>
       <c r="B12" s="110"/>
       <c r="C12" s="111" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="D12" s="111" t="s">
         <v>216</v>
@@ -5105,7 +5105,7 @@
         <v>219</v>
       </c>
       <c r="F12" s="96" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="G12" s="96"/>
       <c r="H12" s="96"/>
@@ -5144,20 +5144,20 @@
       <c r="P13" s="96"/>
       <c r="Q13" s="96"/>
     </row>
-    <row r="14" spans="1:23" s="108" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:23" s="108" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A14" s="109"/>
       <c r="B14" s="110"/>
       <c r="C14" s="111" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="D14" s="111" t="s">
         <v>217</v>
       </c>
       <c r="E14" s="96" t="s">
-        <v>220</v>
+        <v>245</v>
       </c>
       <c r="F14" s="96" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="G14" s="96"/>
       <c r="H14" s="96"/>
@@ -5201,7 +5201,7 @@
         <v>3</v>
       </c>
       <c r="B16" s="105" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="C16" s="106" t="s">
         <v>12</v>
@@ -5213,34 +5213,34 @@
         <v>206</v>
       </c>
       <c r="F16" s="106" t="s">
+        <v>224</v>
+      </c>
+      <c r="G16" s="106" t="s">
         <v>225</v>
       </c>
-      <c r="G16" s="106" t="s">
+      <c r="H16" s="106" t="s">
         <v>226</v>
       </c>
-      <c r="H16" s="106" t="s">
+      <c r="I16" s="106" t="s">
+        <v>238</v>
+      </c>
+      <c r="J16" s="106" t="s">
+        <v>239</v>
+      </c>
+      <c r="K16" s="106" t="s">
         <v>227</v>
       </c>
-      <c r="I16" s="106" t="s">
-        <v>239</v>
-      </c>
-      <c r="J16" s="106" t="s">
-        <v>240</v>
-      </c>
-      <c r="K16" s="106" t="s">
+      <c r="L16" s="106" t="s">
         <v>228</v>
       </c>
-      <c r="L16" s="106" t="s">
+      <c r="M16" s="106" t="s">
         <v>229</v>
       </c>
-      <c r="M16" s="106" t="s">
+      <c r="N16" s="106" t="s">
         <v>230</v>
       </c>
-      <c r="N16" s="106" t="s">
+      <c r="O16" s="106" t="s">
         <v>231</v>
-      </c>
-      <c r="O16" s="106" t="s">
-        <v>232</v>
       </c>
       <c r="P16" s="106"/>
       <c r="Q16" s="106"/>
@@ -5264,34 +5264,34 @@
         <v>208</v>
       </c>
       <c r="F17" s="96" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="G17" s="96" t="s">
+        <v>232</v>
+      </c>
+      <c r="H17" s="96" t="s">
         <v>233</v>
       </c>
-      <c r="H17" s="96" t="s">
-        <v>234</v>
-      </c>
       <c r="I17" s="96" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="J17" s="96" t="s">
         <v>146</v>
       </c>
       <c r="K17" s="96" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="L17" s="96" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="M17" s="96" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="N17" s="118" t="s">
+        <v>236</v>
+      </c>
+      <c r="O17" s="96" t="s">
         <v>237</v>
-      </c>
-      <c r="O17" s="96" t="s">
-        <v>238</v>
       </c>
       <c r="P17" s="96"/>
       <c r="Q17" s="96"/>
@@ -5334,34 +5334,34 @@
         <v>208</v>
       </c>
       <c r="F19" s="96" t="s">
+        <v>241</v>
+      </c>
+      <c r="G19" s="96" t="s">
         <v>242</v>
       </c>
-      <c r="G19" s="96" t="s">
-        <v>243</v>
-      </c>
       <c r="H19" s="96" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="I19" s="96" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="J19" s="96" t="s">
         <v>146</v>
       </c>
       <c r="K19" s="96" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="L19" s="96" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="M19" s="96" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="N19" s="118" t="s">
+        <v>236</v>
+      </c>
+      <c r="O19" s="96" t="s">
         <v>237</v>
-      </c>
-      <c r="O19" s="96" t="s">
-        <v>238</v>
       </c>
       <c r="P19" s="96"/>
       <c r="Q19" s="96"/>

</xml_diff>

<commit_message>
Added Listener. Created New Structure
</commit_message>
<xml_diff>
--- a/src/test/resources/testData/Driver.xlsx
+++ b/src/test/resources/testData/Driver.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19380" windowHeight="6015" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19380" windowHeight="6015" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="TestData_UAT_old" sheetId="15" r:id="rId1"/>
@@ -2623,8 +2623,8 @@
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:AA56"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B28" activeCellId="1" sqref="D27 B28"/>
+    <sheetView topLeftCell="A20" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A22" sqref="A22:XFD22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.3"/>
@@ -4573,8 +4573,8 @@
   <sheetPr codeName="Sheet3"/>
   <dimension ref="A1:F4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4:XFD4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.3"/>
@@ -4787,8 +4787,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:W20"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="84" zoomScaleNormal="84" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+    <sheetView topLeftCell="A2" zoomScale="84" zoomScaleNormal="84" workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Moved Before Method Code to ElementUtil. ScreenShot problem solved
</commit_message>
<xml_diff>
--- a/src/test/resources/testData/Driver.xlsx
+++ b/src/test/resources/testData/Driver.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="69">
   <si>
     <t>Parameteres</t>
   </si>
@@ -225,6 +225,9 @@
   </si>
   <si>
     <t>se</t>
+  </si>
+  <si>
+    <t>no</t>
   </si>
 </sst>
 </file>
@@ -1125,8 +1128,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:W20"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="84" zoomScaleNormal="84" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+    <sheetView tabSelected="1" topLeftCell="A6" zoomScale="84" zoomScaleNormal="84" workbookViewId="0">
+      <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1245,7 +1248,7 @@
       <c r="A5" s="26"/>
       <c r="B5" s="27"/>
       <c r="C5" s="28" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="D5" s="28" t="s">
         <v>33</v>
@@ -1295,7 +1298,7 @@
       <c r="A7" s="26"/>
       <c r="B7" s="27"/>
       <c r="C7" s="28" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="D7" s="28" t="s">
         <v>30</v>
@@ -1382,7 +1385,7 @@
       <c r="A10" s="26"/>
       <c r="B10" s="27"/>
       <c r="C10" s="28" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="D10" s="28" t="s">
         <v>37</v>
@@ -1434,7 +1437,7 @@
       <c r="A12" s="26"/>
       <c r="B12" s="27"/>
       <c r="C12" s="28" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="D12" s="28" t="s">
         <v>38</v>
@@ -1486,7 +1489,7 @@
       <c r="A14" s="26"/>
       <c r="B14" s="27"/>
       <c r="C14" s="28" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="D14" s="28" t="s">
         <v>39</v>
@@ -1663,7 +1666,7 @@
       <c r="A19" s="26"/>
       <c r="B19" s="27"/>
       <c r="C19" s="28" t="s">
-        <v>6</v>
+        <v>68</v>
       </c>
       <c r="D19" s="28" t="s">
         <v>30</v>

</xml_diff>

<commit_message>
Data Sheet For AP added
</commit_message>
<xml_diff>
--- a/src/test/resources/testData/Driver.xlsx
+++ b/src/test/resources/testData/Driver.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="35">
   <si>
     <t>Parameteres</t>
   </si>
@@ -98,9 +98,6 @@
     <t>UAT</t>
   </si>
   <si>
-    <t>1</t>
-  </si>
-  <si>
     <t>varWT</t>
   </si>
   <si>
@@ -125,106 +122,7 @@
     <t>rautsumit2</t>
   </si>
   <si>
-    <t>myCase2</t>
-  </si>
-  <si>
-    <t>team</t>
-  </si>
-  <si>
-    <t>role</t>
-  </si>
-  <si>
-    <t>anika</t>
-  </si>
-  <si>
-    <t>ketki</t>
-  </si>
-  <si>
-    <t>sumt</t>
-  </si>
-  <si>
-    <t>CEO</t>
-  </si>
-  <si>
-    <t>CTO</t>
-  </si>
-  <si>
-    <t>salary</t>
-  </si>
-  <si>
-    <t>1000000</t>
-  </si>
-  <si>
-    <t>1500000</t>
-  </si>
-  <si>
-    <t>10000</t>
-  </si>
-  <si>
-    <t>type</t>
-  </si>
-  <si>
-    <t>passengers</t>
-  </si>
-  <si>
-    <t>departing_from</t>
-  </si>
-  <si>
-    <t>arriving_in</t>
-  </si>
-  <si>
-    <t>returning_month</t>
-  </si>
-  <si>
-    <t>returning_day</t>
-  </si>
-  <si>
-    <t>preferences</t>
-  </si>
-  <si>
-    <t>airline</t>
-  </si>
-  <si>
-    <t>2</t>
-  </si>
-  <si>
-    <t>London</t>
-  </si>
-  <si>
-    <t xml:space="preserve">New yok </t>
-  </si>
-  <si>
-    <t>June</t>
-  </si>
-  <si>
-    <t>Business class</t>
-  </si>
-  <si>
-    <t>Unified Airlines</t>
-  </si>
-  <si>
-    <t>departing_month</t>
-  </si>
-  <si>
-    <t>departing_day</t>
-  </si>
-  <si>
-    <t>WT_Register</t>
-  </si>
-  <si>
-    <t>na</t>
-  </si>
-  <si>
-    <t>3</t>
-  </si>
-  <si>
-    <t>6</t>
-  </si>
-  <si>
     <t>yes</t>
-  </si>
-  <si>
-    <t>se</t>
   </si>
   <si>
     <t>no</t>
@@ -234,7 +132,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -283,12 +181,6 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <sz val="12"/>
-      <color rgb="FF000000"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
   </fonts>
   <fills count="6">
     <fill>
@@ -455,7 +347,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="38">
+  <cellXfs count="37">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -533,7 +425,6 @@
     <xf numFmtId="49" fontId="5" fillId="4" borderId="8" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="49" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="3" fillId="3" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
@@ -934,7 +825,7 @@
         <v>3</v>
       </c>
       <c r="B1" s="14" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C1" s="14" t="s">
         <v>15</v>
@@ -954,7 +845,7 @@
         <v>11</v>
       </c>
       <c r="B2" s="19" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C2" s="10" t="s">
         <v>16</v>
@@ -974,7 +865,7 @@
         <v>12</v>
       </c>
       <c r="B3" s="19" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C3" s="10" t="s">
         <v>16</v>
@@ -994,7 +885,7 @@
         <v>24</v>
       </c>
       <c r="B4" s="19" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C4" s="10" t="s">
         <v>16</v>
@@ -1066,7 +957,7 @@
         <v>5</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
@@ -1126,19 +1017,19 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:W20"/>
+  <dimension ref="A1:W8"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" zoomScale="84" zoomScaleNormal="84" workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
+    <sheetView tabSelected="1" topLeftCell="A8" zoomScale="84" zoomScaleNormal="84" workbookViewId="0">
+      <selection activeCell="A9" sqref="A9:XFD25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="6" width="9.140625" style="36"/>
-    <col min="7" max="7" width="10.7109375" style="36" bestFit="1" customWidth="1"/>
-    <col min="8" max="13" width="9.140625" style="36"/>
-    <col min="14" max="14" width="16.42578125" style="36" bestFit="1" customWidth="1"/>
-    <col min="15" max="16384" width="9.140625" style="36"/>
+    <col min="1" max="6" width="9.140625" style="35"/>
+    <col min="7" max="7" width="10.7109375" style="35" bestFit="1" customWidth="1"/>
+    <col min="8" max="13" width="9.140625" style="35"/>
+    <col min="14" max="14" width="16.42578125" style="35" bestFit="1" customWidth="1"/>
+    <col min="15" max="16384" width="9.140625" style="35"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:23" s="21" customFormat="1" ht="90" x14ac:dyDescent="0.3">
@@ -1148,32 +1039,32 @@
       <c r="B1" s="20" t="s">
         <v>7</v>
       </c>
-      <c r="C1" s="37" t="s">
+      <c r="C1" s="36" t="s">
         <v>0</v>
       </c>
-      <c r="D1" s="37"/>
-      <c r="E1" s="37"/>
-      <c r="F1" s="37"/>
-      <c r="G1" s="37"/>
-      <c r="H1" s="37"/>
-      <c r="I1" s="37"/>
-      <c r="J1" s="37"/>
+      <c r="D1" s="36"/>
+      <c r="E1" s="36"/>
+      <c r="F1" s="36"/>
+      <c r="G1" s="36"/>
+      <c r="H1" s="36"/>
+      <c r="I1" s="36"/>
+      <c r="J1" s="36"/>
     </row>
     <row r="2" spans="1:23" s="25" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A2" s="22">
         <v>1</v>
       </c>
       <c r="B2" s="22" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C2" s="23" t="s">
         <v>10</v>
       </c>
       <c r="D2" s="23" t="s">
+        <v>27</v>
+      </c>
+      <c r="E2" s="23" t="s">
         <v>28</v>
-      </c>
-      <c r="E2" s="23" t="s">
-        <v>29</v>
       </c>
       <c r="F2" s="23"/>
       <c r="G2" s="23"/>
@@ -1198,13 +1089,13 @@
       <c r="A3" s="26"/>
       <c r="B3" s="27"/>
       <c r="C3" s="28" t="s">
-        <v>66</v>
+        <v>33</v>
       </c>
       <c r="D3" s="28" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="E3" s="18" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F3" s="18"/>
       <c r="G3" s="18"/>
@@ -1248,13 +1139,13 @@
       <c r="A5" s="26"/>
       <c r="B5" s="27"/>
       <c r="C5" s="28" t="s">
-        <v>68</v>
+        <v>34</v>
       </c>
       <c r="D5" s="28" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E5" s="18" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F5" s="18"/>
       <c r="G5" s="18"/>
@@ -1298,13 +1189,13 @@
       <c r="A7" s="26"/>
       <c r="B7" s="27"/>
       <c r="C7" s="28" t="s">
-        <v>68</v>
+        <v>34</v>
       </c>
       <c r="D7" s="28" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="E7" s="18" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F7" s="18"/>
       <c r="G7" s="18"/>
@@ -1344,400 +1235,12 @@
       <c r="P8" s="18"/>
       <c r="Q8" s="18"/>
     </row>
-    <row r="9" spans="1:23" s="25" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="22">
-        <v>2</v>
-      </c>
-      <c r="B9" s="22" t="s">
-        <v>34</v>
-      </c>
-      <c r="C9" s="23" t="s">
-        <v>10</v>
-      </c>
-      <c r="D9" s="23" t="s">
-        <v>35</v>
-      </c>
-      <c r="E9" s="23" t="s">
-        <v>36</v>
-      </c>
-      <c r="F9" s="23" t="s">
-        <v>42</v>
-      </c>
-      <c r="G9" s="23"/>
-      <c r="H9" s="23"/>
-      <c r="I9" s="23"/>
-      <c r="J9" s="23"/>
-      <c r="K9" s="23"/>
-      <c r="L9" s="23"/>
-      <c r="M9" s="23"/>
-      <c r="N9" s="23"/>
-      <c r="O9" s="23"/>
-      <c r="P9" s="23"/>
-      <c r="Q9" s="23"/>
-      <c r="R9" s="23"/>
-      <c r="S9" s="23"/>
-      <c r="T9" s="23"/>
-      <c r="U9" s="23"/>
-      <c r="V9" s="24"/>
-      <c r="W9" s="24"/>
-    </row>
-    <row r="10" spans="1:23" s="25" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="26"/>
-      <c r="B10" s="27"/>
-      <c r="C10" s="28" t="s">
-        <v>68</v>
-      </c>
-      <c r="D10" s="28" t="s">
-        <v>37</v>
-      </c>
-      <c r="E10" s="18" t="s">
-        <v>40</v>
-      </c>
-      <c r="F10" s="18" t="s">
-        <v>43</v>
-      </c>
-      <c r="G10" s="18"/>
-      <c r="H10" s="18"/>
-      <c r="I10" s="18"/>
-      <c r="J10" s="18"/>
-      <c r="K10" s="18"/>
-      <c r="L10" s="18"/>
-      <c r="M10" s="29"/>
-      <c r="N10" s="29"/>
-      <c r="O10" s="18"/>
-      <c r="P10" s="18"/>
-      <c r="Q10" s="18"/>
-      <c r="R10" s="18"/>
-      <c r="S10" s="23"/>
-      <c r="T10" s="30"/>
-      <c r="U10" s="23"/>
-      <c r="V10" s="24"/>
-      <c r="W10" s="24"/>
-    </row>
-    <row r="11" spans="1:23" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="31"/>
-      <c r="B11" s="27"/>
-      <c r="C11" s="28"/>
-      <c r="D11" s="18"/>
-      <c r="E11" s="18"/>
-      <c r="F11" s="18"/>
-      <c r="G11" s="29"/>
-      <c r="H11" s="32"/>
-      <c r="I11" s="33"/>
-      <c r="J11" s="33"/>
-      <c r="K11" s="18"/>
-      <c r="L11" s="34"/>
-      <c r="M11" s="18"/>
-      <c r="N11" s="18"/>
-      <c r="O11" s="18"/>
-      <c r="P11" s="18"/>
-      <c r="Q11" s="18"/>
-    </row>
-    <row r="12" spans="1:23" s="25" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="26"/>
-      <c r="B12" s="27"/>
-      <c r="C12" s="28" t="s">
-        <v>68</v>
-      </c>
-      <c r="D12" s="28" t="s">
-        <v>38</v>
-      </c>
-      <c r="E12" s="18" t="s">
-        <v>41</v>
-      </c>
-      <c r="F12" s="18" t="s">
-        <v>44</v>
-      </c>
-      <c r="G12" s="18"/>
-      <c r="H12" s="18"/>
-      <c r="I12" s="18"/>
-      <c r="J12" s="18"/>
-      <c r="K12" s="18"/>
-      <c r="L12" s="18"/>
-      <c r="M12" s="29"/>
-      <c r="N12" s="29"/>
-      <c r="O12" s="18"/>
-      <c r="P12" s="18"/>
-      <c r="Q12" s="18"/>
-      <c r="R12" s="18"/>
-      <c r="S12" s="23"/>
-      <c r="T12" s="30"/>
-      <c r="U12" s="23"/>
-      <c r="V12" s="24"/>
-      <c r="W12" s="24"/>
-    </row>
-    <row r="13" spans="1:23" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="31"/>
-      <c r="B13" s="27"/>
-      <c r="C13" s="28"/>
-      <c r="D13" s="18"/>
-      <c r="E13" s="18"/>
-      <c r="F13" s="18"/>
-      <c r="G13" s="29"/>
-      <c r="H13" s="32"/>
-      <c r="I13" s="33"/>
-      <c r="J13" s="33"/>
-      <c r="K13" s="18"/>
-      <c r="L13" s="34"/>
-      <c r="M13" s="18"/>
-      <c r="N13" s="18"/>
-      <c r="O13" s="18"/>
-      <c r="P13" s="18"/>
-      <c r="Q13" s="18"/>
-    </row>
-    <row r="14" spans="1:23" s="25" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="26"/>
-      <c r="B14" s="27"/>
-      <c r="C14" s="28" t="s">
-        <v>68</v>
-      </c>
-      <c r="D14" s="28" t="s">
-        <v>39</v>
-      </c>
-      <c r="E14" s="18" t="s">
-        <v>67</v>
-      </c>
-      <c r="F14" s="18" t="s">
-        <v>45</v>
-      </c>
-      <c r="G14" s="18"/>
-      <c r="H14" s="18"/>
-      <c r="I14" s="18"/>
-      <c r="J14" s="18"/>
-      <c r="K14" s="18"/>
-      <c r="L14" s="18"/>
-      <c r="M14" s="29"/>
-      <c r="N14" s="29"/>
-      <c r="O14" s="18"/>
-      <c r="P14" s="18"/>
-      <c r="Q14" s="18"/>
-      <c r="R14" s="18"/>
-      <c r="S14" s="23"/>
-      <c r="T14" s="30"/>
-      <c r="U14" s="23"/>
-      <c r="V14" s="24"/>
-      <c r="W14" s="24"/>
-    </row>
-    <row r="15" spans="1:23" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="31"/>
-      <c r="B15" s="27"/>
-      <c r="C15" s="28"/>
-      <c r="D15" s="18"/>
-      <c r="E15" s="18"/>
-      <c r="F15" s="18"/>
-      <c r="G15" s="29"/>
-      <c r="H15" s="32"/>
-      <c r="I15" s="33"/>
-      <c r="J15" s="33"/>
-      <c r="K15" s="18"/>
-      <c r="L15" s="34"/>
-      <c r="M15" s="18"/>
-      <c r="N15" s="18"/>
-      <c r="O15" s="18"/>
-      <c r="P15" s="18"/>
-      <c r="Q15" s="18"/>
-    </row>
-    <row r="16" spans="1:23" s="25" customFormat="1" ht="30" x14ac:dyDescent="0.3">
-      <c r="A16" s="22">
-        <v>3</v>
-      </c>
-      <c r="B16" s="22" t="s">
-        <v>62</v>
-      </c>
-      <c r="C16" s="23" t="s">
-        <v>10</v>
-      </c>
-      <c r="D16" s="23" t="s">
-        <v>28</v>
-      </c>
-      <c r="E16" s="23" t="s">
-        <v>29</v>
-      </c>
-      <c r="F16" s="23" t="s">
-        <v>46</v>
-      </c>
-      <c r="G16" s="23" t="s">
-        <v>47</v>
-      </c>
-      <c r="H16" s="23" t="s">
-        <v>48</v>
-      </c>
-      <c r="I16" s="23" t="s">
-        <v>60</v>
-      </c>
-      <c r="J16" s="23" t="s">
-        <v>61</v>
-      </c>
-      <c r="K16" s="23" t="s">
-        <v>49</v>
-      </c>
-      <c r="L16" s="23" t="s">
-        <v>50</v>
-      </c>
-      <c r="M16" s="23" t="s">
-        <v>51</v>
-      </c>
-      <c r="N16" s="23" t="s">
-        <v>52</v>
-      </c>
-      <c r="O16" s="23" t="s">
-        <v>53</v>
-      </c>
-      <c r="P16" s="23"/>
-      <c r="Q16" s="23"/>
-      <c r="R16" s="23"/>
-      <c r="S16" s="23"/>
-      <c r="T16" s="23"/>
-      <c r="U16" s="23"/>
-      <c r="V16" s="24"/>
-      <c r="W16" s="24"/>
-    </row>
-    <row r="17" spans="1:23" s="25" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A17" s="26"/>
-      <c r="B17" s="27"/>
-      <c r="C17" s="28" t="s">
-        <v>6</v>
-      </c>
-      <c r="D17" s="28" t="s">
-        <v>30</v>
-      </c>
-      <c r="E17" s="18" t="s">
-        <v>30</v>
-      </c>
-      <c r="F17" s="18" t="s">
-        <v>63</v>
-      </c>
-      <c r="G17" s="18" t="s">
-        <v>54</v>
-      </c>
-      <c r="H17" s="18" t="s">
-        <v>55</v>
-      </c>
-      <c r="I17" s="18" t="s">
-        <v>57</v>
-      </c>
-      <c r="J17" s="18" t="s">
-        <v>25</v>
-      </c>
-      <c r="K17" s="18" t="s">
-        <v>56</v>
-      </c>
-      <c r="L17" s="18" t="s">
-        <v>65</v>
-      </c>
-      <c r="M17" s="18" t="s">
-        <v>64</v>
-      </c>
-      <c r="N17" s="35" t="s">
-        <v>58</v>
-      </c>
-      <c r="O17" s="18" t="s">
-        <v>59</v>
-      </c>
-      <c r="P17" s="18"/>
-      <c r="Q17" s="18"/>
-      <c r="R17" s="18"/>
-      <c r="S17" s="23"/>
-      <c r="T17" s="30"/>
-      <c r="U17" s="23"/>
-      <c r="V17" s="24"/>
-      <c r="W17" s="24"/>
-    </row>
-    <row r="18" spans="1:23" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="31"/>
-      <c r="B18" s="27"/>
-      <c r="C18" s="28"/>
-      <c r="D18" s="18"/>
-      <c r="E18" s="18"/>
-      <c r="F18" s="18"/>
-      <c r="G18" s="29"/>
-      <c r="H18" s="32"/>
-      <c r="I18" s="33"/>
-      <c r="J18" s="33"/>
-      <c r="K18" s="18"/>
-      <c r="L18" s="34"/>
-      <c r="M18" s="18"/>
-      <c r="N18" s="18"/>
-      <c r="O18" s="18"/>
-      <c r="P18" s="18"/>
-      <c r="Q18" s="18"/>
-    </row>
-    <row r="19" spans="1:23" s="25" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A19" s="26"/>
-      <c r="B19" s="27"/>
-      <c r="C19" s="28" t="s">
-        <v>68</v>
-      </c>
-      <c r="D19" s="28" t="s">
-        <v>30</v>
-      </c>
-      <c r="E19" s="18" t="s">
-        <v>30</v>
-      </c>
-      <c r="F19" s="18" t="s">
-        <v>63</v>
-      </c>
-      <c r="G19" s="18" t="s">
-        <v>64</v>
-      </c>
-      <c r="H19" s="18" t="s">
-        <v>55</v>
-      </c>
-      <c r="I19" s="18" t="s">
-        <v>57</v>
-      </c>
-      <c r="J19" s="18" t="s">
-        <v>25</v>
-      </c>
-      <c r="K19" s="18" t="s">
-        <v>56</v>
-      </c>
-      <c r="L19" s="18" t="s">
-        <v>65</v>
-      </c>
-      <c r="M19" s="18" t="s">
-        <v>64</v>
-      </c>
-      <c r="N19" s="35" t="s">
-        <v>58</v>
-      </c>
-      <c r="O19" s="18" t="s">
-        <v>59</v>
-      </c>
-      <c r="P19" s="18"/>
-      <c r="Q19" s="18"/>
-      <c r="R19" s="18"/>
-      <c r="S19" s="23"/>
-      <c r="T19" s="30"/>
-      <c r="U19" s="23"/>
-      <c r="V19" s="24"/>
-      <c r="W19" s="24"/>
-    </row>
-    <row r="20" spans="1:23" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="31"/>
-      <c r="B20" s="27"/>
-      <c r="C20" s="28"/>
-      <c r="D20" s="18"/>
-      <c r="E20" s="18"/>
-      <c r="F20" s="18"/>
-      <c r="G20" s="29"/>
-      <c r="H20" s="32"/>
-      <c r="I20" s="33"/>
-      <c r="J20" s="33"/>
-      <c r="K20" s="18"/>
-      <c r="L20" s="34"/>
-      <c r="M20" s="18"/>
-      <c r="N20" s="18"/>
-      <c r="O20" s="18"/>
-      <c r="P20" s="18"/>
-      <c r="Q20" s="18"/>
-    </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="C1:J1"/>
   </mergeCells>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" sqref="L1:L16 L18 L20">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" sqref="L1:L8">
       <formula1>"5000,,7000,,8000"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
Added test classes to AT Project
</commit_message>
<xml_diff>
--- a/src/test/resources/testData/Driver.xlsx
+++ b/src/test/resources/testData/Driver.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="37">
   <si>
     <t>Parameteres</t>
   </si>
@@ -101,15 +101,6 @@
     <t>varWT</t>
   </si>
   <si>
-    <t>myCase</t>
-  </si>
-  <si>
-    <t>username</t>
-  </si>
-  <si>
-    <t>password</t>
-  </si>
-  <si>
     <t>rautsumit</t>
   </si>
   <si>
@@ -126,6 +117,21 @@
   </si>
   <si>
     <t>no</t>
+  </si>
+  <si>
+    <t>AT_01_NewAccount</t>
+  </si>
+  <si>
+    <t>emailaddress</t>
+  </si>
+  <si>
+    <t>gender</t>
+  </si>
+  <si>
+    <t>male</t>
+  </si>
+  <si>
+    <t>rautsumit@test.com</t>
   </si>
 </sst>
 </file>
@@ -347,7 +353,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="37">
+  <cellXfs count="38">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -387,9 +393,6 @@
     <xf numFmtId="49" fontId="4" fillId="3" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="3" fillId="3" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
     <xf numFmtId="49" fontId="3" fillId="4" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="3" fillId="4" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -428,6 +431,12 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="3" fillId="3" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="3" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="4" borderId="8" xfId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -845,7 +854,7 @@
         <v>11</v>
       </c>
       <c r="B2" s="19" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="C2" s="10" t="s">
         <v>16</v>
@@ -865,7 +874,7 @@
         <v>12</v>
       </c>
       <c r="B3" s="19" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="C3" s="10" t="s">
         <v>16</v>
@@ -885,7 +894,7 @@
         <v>24</v>
       </c>
       <c r="B4" s="19" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="C4" s="10" t="s">
         <v>16</v>
@@ -957,7 +966,7 @@
         <v>5</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
@@ -1019,20 +1028,22 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:W8"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" zoomScale="84" zoomScaleNormal="84" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9:XFD25"/>
+    <sheetView tabSelected="1" zoomScale="84" zoomScaleNormal="84" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="6" width="9.140625" style="35"/>
-    <col min="7" max="7" width="10.7109375" style="35" bestFit="1" customWidth="1"/>
-    <col min="8" max="13" width="9.140625" style="35"/>
-    <col min="14" max="14" width="16.42578125" style="35" bestFit="1" customWidth="1"/>
-    <col min="15" max="16384" width="9.140625" style="35"/>
+    <col min="1" max="1" width="9.140625" style="34"/>
+    <col min="2" max="2" width="18.140625" style="34" bestFit="1" customWidth="1"/>
+    <col min="3" max="6" width="9.140625" style="34"/>
+    <col min="7" max="7" width="10.7109375" style="34" bestFit="1" customWidth="1"/>
+    <col min="8" max="13" width="9.140625" style="34"/>
+    <col min="14" max="14" width="16.42578125" style="34" bestFit="1" customWidth="1"/>
+    <col min="15" max="16384" width="9.140625" style="34"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:23" s="21" customFormat="1" ht="90" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:23" s="35" customFormat="1" ht="45" x14ac:dyDescent="0.3">
       <c r="A1" s="20" t="s">
         <v>4</v>
       </c>
@@ -1050,52 +1061,52 @@
       <c r="I1" s="36"/>
       <c r="J1" s="36"/>
     </row>
-    <row r="2" spans="1:23" s="25" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="22">
+    <row r="2" spans="1:23" s="24" customFormat="1" ht="30" x14ac:dyDescent="0.3">
+      <c r="A2" s="21">
         <v>1</v>
       </c>
-      <c r="B2" s="22" t="s">
-        <v>26</v>
-      </c>
-      <c r="C2" s="23" t="s">
+      <c r="B2" s="21" t="s">
+        <v>32</v>
+      </c>
+      <c r="C2" s="22" t="s">
         <v>10</v>
       </c>
-      <c r="D2" s="23" t="s">
-        <v>27</v>
-      </c>
-      <c r="E2" s="23" t="s">
-        <v>28</v>
-      </c>
-      <c r="F2" s="23"/>
-      <c r="G2" s="23"/>
-      <c r="H2" s="23"/>
-      <c r="I2" s="23"/>
-      <c r="J2" s="23"/>
-      <c r="K2" s="23"/>
-      <c r="L2" s="23"/>
-      <c r="M2" s="23"/>
-      <c r="N2" s="23"/>
-      <c r="O2" s="23"/>
-      <c r="P2" s="23"/>
-      <c r="Q2" s="23"/>
-      <c r="R2" s="23"/>
-      <c r="S2" s="23"/>
-      <c r="T2" s="23"/>
-      <c r="U2" s="23"/>
-      <c r="V2" s="24"/>
-      <c r="W2" s="24"/>
-    </row>
-    <row r="3" spans="1:23" s="25" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A3" s="26"/>
-      <c r="B3" s="27"/>
-      <c r="C3" s="28" t="s">
+      <c r="D2" s="22" t="s">
         <v>33</v>
       </c>
-      <c r="D3" s="28" t="s">
-        <v>29</v>
+      <c r="E2" s="22" t="s">
+        <v>34</v>
+      </c>
+      <c r="F2" s="22"/>
+      <c r="G2" s="22"/>
+      <c r="H2" s="22"/>
+      <c r="I2" s="22"/>
+      <c r="J2" s="22"/>
+      <c r="K2" s="22"/>
+      <c r="L2" s="22"/>
+      <c r="M2" s="22"/>
+      <c r="N2" s="22"/>
+      <c r="O2" s="22"/>
+      <c r="P2" s="22"/>
+      <c r="Q2" s="22"/>
+      <c r="R2" s="22"/>
+      <c r="S2" s="22"/>
+      <c r="T2" s="22"/>
+      <c r="U2" s="22"/>
+      <c r="V2" s="23"/>
+      <c r="W2" s="23"/>
+    </row>
+    <row r="3" spans="1:23" s="24" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+      <c r="A3" s="25"/>
+      <c r="B3" s="26"/>
+      <c r="C3" s="27" t="s">
+        <v>30</v>
+      </c>
+      <c r="D3" s="37" t="s">
+        <v>36</v>
       </c>
       <c r="E3" s="18" t="s">
-        <v>29</v>
+        <v>35</v>
       </c>
       <c r="F3" s="18"/>
       <c r="G3" s="18"/>
@@ -1104,48 +1115,48 @@
       <c r="J3" s="18"/>
       <c r="K3" s="18"/>
       <c r="L3" s="18"/>
-      <c r="M3" s="29"/>
-      <c r="N3" s="29"/>
+      <c r="M3" s="28"/>
+      <c r="N3" s="28"/>
       <c r="O3" s="18"/>
       <c r="P3" s="18"/>
       <c r="Q3" s="18"/>
       <c r="R3" s="18"/>
-      <c r="S3" s="23"/>
-      <c r="T3" s="30"/>
-      <c r="U3" s="23"/>
-      <c r="V3" s="24"/>
-      <c r="W3" s="24"/>
-    </row>
-    <row r="4" spans="1:23" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="31"/>
-      <c r="B4" s="27"/>
-      <c r="C4" s="28"/>
+      <c r="S3" s="22"/>
+      <c r="T3" s="29"/>
+      <c r="U3" s="22"/>
+      <c r="V3" s="23"/>
+      <c r="W3" s="23"/>
+    </row>
+    <row r="4" spans="1:23" s="22" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="30"/>
+      <c r="B4" s="26"/>
+      <c r="C4" s="27"/>
       <c r="D4" s="18"/>
       <c r="E4" s="18"/>
       <c r="F4" s="18"/>
-      <c r="G4" s="29"/>
-      <c r="H4" s="32"/>
-      <c r="I4" s="33"/>
-      <c r="J4" s="33"/>
+      <c r="G4" s="28"/>
+      <c r="H4" s="31"/>
+      <c r="I4" s="32"/>
+      <c r="J4" s="32"/>
       <c r="K4" s="18"/>
-      <c r="L4" s="34"/>
+      <c r="L4" s="33"/>
       <c r="M4" s="18"/>
       <c r="N4" s="18"/>
       <c r="O4" s="18"/>
       <c r="P4" s="18"/>
       <c r="Q4" s="18"/>
     </row>
-    <row r="5" spans="1:23" s="25" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A5" s="26"/>
-      <c r="B5" s="27"/>
-      <c r="C5" s="28" t="s">
-        <v>34</v>
-      </c>
-      <c r="D5" s="28" t="s">
-        <v>32</v>
+    <row r="5" spans="1:23" s="24" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A5" s="25"/>
+      <c r="B5" s="26"/>
+      <c r="C5" s="27" t="s">
+        <v>31</v>
+      </c>
+      <c r="D5" s="27" t="s">
+        <v>29</v>
       </c>
       <c r="E5" s="18" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="F5" s="18"/>
       <c r="G5" s="18"/>
@@ -1154,48 +1165,48 @@
       <c r="J5" s="18"/>
       <c r="K5" s="18"/>
       <c r="L5" s="18"/>
-      <c r="M5" s="29"/>
-      <c r="N5" s="29"/>
+      <c r="M5" s="28"/>
+      <c r="N5" s="28"/>
       <c r="O5" s="18"/>
       <c r="P5" s="18"/>
       <c r="Q5" s="18"/>
       <c r="R5" s="18"/>
-      <c r="S5" s="23"/>
-      <c r="T5" s="30"/>
-      <c r="U5" s="23"/>
-      <c r="V5" s="24"/>
-      <c r="W5" s="24"/>
-    </row>
-    <row r="6" spans="1:23" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="31"/>
-      <c r="B6" s="27"/>
-      <c r="C6" s="28"/>
+      <c r="S5" s="22"/>
+      <c r="T5" s="29"/>
+      <c r="U5" s="22"/>
+      <c r="V5" s="23"/>
+      <c r="W5" s="23"/>
+    </row>
+    <row r="6" spans="1:23" s="22" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="30"/>
+      <c r="B6" s="26"/>
+      <c r="C6" s="27"/>
       <c r="D6" s="18"/>
       <c r="E6" s="18"/>
       <c r="F6" s="18"/>
-      <c r="G6" s="29"/>
-      <c r="H6" s="32"/>
-      <c r="I6" s="33"/>
-      <c r="J6" s="33"/>
+      <c r="G6" s="28"/>
+      <c r="H6" s="31"/>
+      <c r="I6" s="32"/>
+      <c r="J6" s="32"/>
       <c r="K6" s="18"/>
-      <c r="L6" s="34"/>
+      <c r="L6" s="33"/>
       <c r="M6" s="18"/>
       <c r="N6" s="18"/>
       <c r="O6" s="18"/>
       <c r="P6" s="18"/>
       <c r="Q6" s="18"/>
     </row>
-    <row r="7" spans="1:23" s="25" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A7" s="26"/>
-      <c r="B7" s="27"/>
-      <c r="C7" s="28" t="s">
-        <v>34</v>
-      </c>
-      <c r="D7" s="28" t="s">
-        <v>29</v>
+    <row r="7" spans="1:23" s="24" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A7" s="25"/>
+      <c r="B7" s="26"/>
+      <c r="C7" s="27" t="s">
+        <v>31</v>
+      </c>
+      <c r="D7" s="27" t="s">
+        <v>26</v>
       </c>
       <c r="E7" s="18" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="F7" s="18"/>
       <c r="G7" s="18"/>
@@ -1204,31 +1215,31 @@
       <c r="J7" s="18"/>
       <c r="K7" s="18"/>
       <c r="L7" s="18"/>
-      <c r="M7" s="29"/>
-      <c r="N7" s="29"/>
+      <c r="M7" s="28"/>
+      <c r="N7" s="28"/>
       <c r="O7" s="18"/>
       <c r="P7" s="18"/>
       <c r="Q7" s="18"/>
       <c r="R7" s="18"/>
-      <c r="S7" s="23"/>
-      <c r="T7" s="30"/>
-      <c r="U7" s="23"/>
-      <c r="V7" s="24"/>
-      <c r="W7" s="24"/>
-    </row>
-    <row r="8" spans="1:23" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="31"/>
-      <c r="B8" s="27"/>
-      <c r="C8" s="28"/>
+      <c r="S7" s="22"/>
+      <c r="T7" s="29"/>
+      <c r="U7" s="22"/>
+      <c r="V7" s="23"/>
+      <c r="W7" s="23"/>
+    </row>
+    <row r="8" spans="1:23" s="22" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="30"/>
+      <c r="B8" s="26"/>
+      <c r="C8" s="27"/>
       <c r="D8" s="18"/>
       <c r="E8" s="18"/>
       <c r="F8" s="18"/>
-      <c r="G8" s="29"/>
-      <c r="H8" s="32"/>
-      <c r="I8" s="33"/>
-      <c r="J8" s="33"/>
+      <c r="G8" s="28"/>
+      <c r="H8" s="31"/>
+      <c r="I8" s="32"/>
+      <c r="J8" s="32"/>
       <c r="K8" s="18"/>
-      <c r="L8" s="34"/>
+      <c r="L8" s="33"/>
       <c r="M8" s="18"/>
       <c r="N8" s="18"/>
       <c r="O8" s="18"/>
@@ -1244,7 +1255,10 @@
       <formula1>"5000,,7000,,8000"</formula1>
     </dataValidation>
   </dataValidations>
+  <hyperlinks>
+    <hyperlink ref="D3" r:id="rId1"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Added WT testcases with element util modification
</commit_message>
<xml_diff>
--- a/src/test/resources/testData/Driver.xlsx
+++ b/src/test/resources/testData/Driver.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="42">
   <si>
     <t>Parameteres</t>
   </si>
@@ -101,6 +101,9 @@
     <t>varWT</t>
   </si>
   <si>
+    <t>password</t>
+  </si>
+  <si>
     <t>rautsumit</t>
   </si>
   <si>
@@ -110,9 +113,6 @@
     <t>WebTours</t>
   </si>
   <si>
-    <t>rautsumit2</t>
-  </si>
-  <si>
     <t>yes</t>
   </si>
   <si>
@@ -132,6 +132,21 @@
   </si>
   <si>
     <t>rautsumit@test.com</t>
+  </si>
+  <si>
+    <t>firstname</t>
+  </si>
+  <si>
+    <t>lastname</t>
+  </si>
+  <si>
+    <t>sumit</t>
+  </si>
+  <si>
+    <t>raut</t>
+  </si>
+  <si>
+    <t>pwd</t>
   </si>
 </sst>
 </file>
@@ -854,7 +869,7 @@
         <v>11</v>
       </c>
       <c r="B2" s="19" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="C2" s="10" t="s">
         <v>16</v>
@@ -874,7 +889,7 @@
         <v>12</v>
       </c>
       <c r="B3" s="19" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="C3" s="10" t="s">
         <v>16</v>
@@ -894,7 +909,7 @@
         <v>24</v>
       </c>
       <c r="B4" s="19" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="C4" s="10" t="s">
         <v>16</v>
@@ -966,7 +981,7 @@
         <v>5</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
@@ -1029,7 +1044,7 @@
   <dimension ref="A1:W8"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="84" zoomScaleNormal="84" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="A5" sqref="A5:XFD5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1077,9 +1092,15 @@
       <c r="E2" s="22" t="s">
         <v>34</v>
       </c>
-      <c r="F2" s="22"/>
-      <c r="G2" s="22"/>
-      <c r="H2" s="22"/>
+      <c r="F2" s="22" t="s">
+        <v>37</v>
+      </c>
+      <c r="G2" s="22" t="s">
+        <v>38</v>
+      </c>
+      <c r="H2" s="22" t="s">
+        <v>26</v>
+      </c>
       <c r="I2" s="22"/>
       <c r="J2" s="22"/>
       <c r="K2" s="22"/>
@@ -1108,9 +1129,15 @@
       <c r="E3" s="18" t="s">
         <v>35</v>
       </c>
-      <c r="F3" s="18"/>
-      <c r="G3" s="18"/>
-      <c r="H3" s="18"/>
+      <c r="F3" s="18" t="s">
+        <v>39</v>
+      </c>
+      <c r="G3" s="18" t="s">
+        <v>40</v>
+      </c>
+      <c r="H3" s="18" t="s">
+        <v>41</v>
+      </c>
       <c r="I3" s="18"/>
       <c r="J3" s="18"/>
       <c r="K3" s="18"/>
@@ -1146,21 +1173,27 @@
       <c r="P4" s="18"/>
       <c r="Q4" s="18"/>
     </row>
-    <row r="5" spans="1:23" s="24" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:23" s="24" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A5" s="25"/>
       <c r="B5" s="26"/>
       <c r="C5" s="27" t="s">
-        <v>31</v>
-      </c>
-      <c r="D5" s="27" t="s">
-        <v>29</v>
+        <v>30</v>
+      </c>
+      <c r="D5" s="37" t="s">
+        <v>36</v>
       </c>
       <c r="E5" s="18" t="s">
-        <v>26</v>
-      </c>
-      <c r="F5" s="18"/>
-      <c r="G5" s="18"/>
-      <c r="H5" s="18"/>
+        <v>35</v>
+      </c>
+      <c r="F5" s="18" t="s">
+        <v>39</v>
+      </c>
+      <c r="G5" s="18" t="s">
+        <v>40</v>
+      </c>
+      <c r="H5" s="18" t="s">
+        <v>41</v>
+      </c>
       <c r="I5" s="18"/>
       <c r="J5" s="18"/>
       <c r="K5" s="18"/>
@@ -1203,10 +1236,10 @@
         <v>31</v>
       </c>
       <c r="D7" s="27" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="E7" s="18" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="F7" s="18"/>
       <c r="G7" s="18"/>
@@ -1257,8 +1290,9 @@
   </dataValidations>
   <hyperlinks>
     <hyperlink ref="D3" r:id="rId1"/>
+    <hyperlink ref="D5" r:id="rId2"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Added WT testcases with element util modification 2
</commit_message>
<xml_diff>
--- a/src/test/resources/testData/Driver.xlsx
+++ b/src/test/resources/testData/Driver.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="42">
   <si>
     <t>Parameteres</t>
   </si>
@@ -116,9 +116,6 @@
     <t>yes</t>
   </si>
   <si>
-    <t>no</t>
-  </si>
-  <si>
     <t>AT_01_NewAccount</t>
   </si>
   <si>
@@ -147,6 +144,9 @@
   </si>
   <si>
     <t>pwd</t>
+  </si>
+  <si>
+    <t>s@s.com</t>
   </si>
 </sst>
 </file>
@@ -447,11 +447,11 @@
     <xf numFmtId="49" fontId="3" fillId="3" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
+    <xf numFmtId="49" fontId="2" fillId="4" borderId="8" xfId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="49" fontId="3" fillId="3" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="4" borderId="8" xfId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1041,10 +1041,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:W8"/>
+  <dimension ref="A1:W12"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="84" zoomScaleNormal="84" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5:XFD5"/>
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1065,38 +1065,38 @@
       <c r="B1" s="20" t="s">
         <v>7</v>
       </c>
-      <c r="C1" s="36" t="s">
+      <c r="C1" s="37" t="s">
         <v>0</v>
       </c>
-      <c r="D1" s="36"/>
-      <c r="E1" s="36"/>
-      <c r="F1" s="36"/>
-      <c r="G1" s="36"/>
-      <c r="H1" s="36"/>
-      <c r="I1" s="36"/>
-      <c r="J1" s="36"/>
+      <c r="D1" s="37"/>
+      <c r="E1" s="37"/>
+      <c r="F1" s="37"/>
+      <c r="G1" s="37"/>
+      <c r="H1" s="37"/>
+      <c r="I1" s="37"/>
+      <c r="J1" s="37"/>
     </row>
     <row r="2" spans="1:23" s="24" customFormat="1" ht="30" x14ac:dyDescent="0.3">
       <c r="A2" s="21">
         <v>1</v>
       </c>
       <c r="B2" s="21" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C2" s="22" t="s">
         <v>10</v>
       </c>
       <c r="D2" s="22" t="s">
+        <v>32</v>
+      </c>
+      <c r="E2" s="22" t="s">
         <v>33</v>
       </c>
-      <c r="E2" s="22" t="s">
-        <v>34</v>
-      </c>
       <c r="F2" s="22" t="s">
+        <v>36</v>
+      </c>
+      <c r="G2" s="22" t="s">
         <v>37</v>
-      </c>
-      <c r="G2" s="22" t="s">
-        <v>38</v>
       </c>
       <c r="H2" s="22" t="s">
         <v>26</v>
@@ -1123,20 +1123,20 @@
       <c r="C3" s="27" t="s">
         <v>30</v>
       </c>
-      <c r="D3" s="37" t="s">
-        <v>36</v>
+      <c r="D3" s="36" t="s">
+        <v>35</v>
       </c>
       <c r="E3" s="18" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="F3" s="18" t="s">
+        <v>38</v>
+      </c>
+      <c r="G3" s="18" t="s">
         <v>39</v>
       </c>
-      <c r="G3" s="18" t="s">
+      <c r="H3" s="18" t="s">
         <v>40</v>
-      </c>
-      <c r="H3" s="18" t="s">
-        <v>41</v>
       </c>
       <c r="I3" s="18"/>
       <c r="J3" s="18"/>
@@ -1179,20 +1179,20 @@
       <c r="C5" s="27" t="s">
         <v>30</v>
       </c>
-      <c r="D5" s="37" t="s">
-        <v>36</v>
+      <c r="D5" s="36" t="s">
+        <v>35</v>
       </c>
       <c r="E5" s="18" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="F5" s="18" t="s">
+        <v>38</v>
+      </c>
+      <c r="G5" s="18" t="s">
         <v>39</v>
       </c>
-      <c r="G5" s="18" t="s">
+      <c r="H5" s="18" t="s">
         <v>40</v>
-      </c>
-      <c r="H5" s="18" t="s">
-        <v>41</v>
       </c>
       <c r="I5" s="18"/>
       <c r="J5" s="18"/>
@@ -1233,17 +1233,23 @@
       <c r="A7" s="25"/>
       <c r="B7" s="26"/>
       <c r="C7" s="27" t="s">
-        <v>31</v>
-      </c>
-      <c r="D7" s="27" t="s">
-        <v>27</v>
+        <v>30</v>
+      </c>
+      <c r="D7" s="36" t="s">
+        <v>41</v>
       </c>
       <c r="E7" s="18" t="s">
         <v>27</v>
       </c>
-      <c r="F7" s="18"/>
-      <c r="G7" s="18"/>
-      <c r="H7" s="18"/>
+      <c r="F7" s="18" t="s">
+        <v>38</v>
+      </c>
+      <c r="G7" s="18" t="s">
+        <v>39</v>
+      </c>
+      <c r="H7" s="18" t="s">
+        <v>40</v>
+      </c>
       <c r="I7" s="18"/>
       <c r="J7" s="18"/>
       <c r="K7" s="18"/>
@@ -1279,20 +1285,135 @@
       <c r="P8" s="18"/>
       <c r="Q8" s="18"/>
     </row>
+    <row r="9" spans="1:23" s="24" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A9" s="25"/>
+      <c r="B9" s="26"/>
+      <c r="C9" s="27" t="s">
+        <v>30</v>
+      </c>
+      <c r="D9" s="36" t="s">
+        <v>41</v>
+      </c>
+      <c r="E9" s="18" t="s">
+        <v>27</v>
+      </c>
+      <c r="F9" s="18" t="s">
+        <v>38</v>
+      </c>
+      <c r="G9" s="18" t="s">
+        <v>39</v>
+      </c>
+      <c r="H9" s="18" t="s">
+        <v>40</v>
+      </c>
+      <c r="I9" s="18"/>
+      <c r="J9" s="18"/>
+      <c r="K9" s="18"/>
+      <c r="L9" s="18"/>
+      <c r="M9" s="28"/>
+      <c r="N9" s="28"/>
+      <c r="O9" s="18"/>
+      <c r="P9" s="18"/>
+      <c r="Q9" s="18"/>
+      <c r="R9" s="18"/>
+      <c r="S9" s="22"/>
+      <c r="T9" s="29"/>
+      <c r="U9" s="22"/>
+      <c r="V9" s="23"/>
+      <c r="W9" s="23"/>
+    </row>
+    <row r="10" spans="1:23" s="22" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="30"/>
+      <c r="B10" s="26"/>
+      <c r="C10" s="27"/>
+      <c r="D10" s="18"/>
+      <c r="E10" s="18"/>
+      <c r="F10" s="18"/>
+      <c r="G10" s="28"/>
+      <c r="H10" s="31"/>
+      <c r="I10" s="32"/>
+      <c r="J10" s="32"/>
+      <c r="K10" s="18"/>
+      <c r="L10" s="33"/>
+      <c r="M10" s="18"/>
+      <c r="N10" s="18"/>
+      <c r="O10" s="18"/>
+      <c r="P10" s="18"/>
+      <c r="Q10" s="18"/>
+    </row>
+    <row r="11" spans="1:23" s="24" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+      <c r="A11" s="25"/>
+      <c r="B11" s="26"/>
+      <c r="C11" s="27" t="s">
+        <v>30</v>
+      </c>
+      <c r="D11" s="36" t="s">
+        <v>35</v>
+      </c>
+      <c r="E11" s="18" t="s">
+        <v>34</v>
+      </c>
+      <c r="F11" s="18" t="s">
+        <v>38</v>
+      </c>
+      <c r="G11" s="18" t="s">
+        <v>39</v>
+      </c>
+      <c r="H11" s="18" t="s">
+        <v>40</v>
+      </c>
+      <c r="I11" s="18"/>
+      <c r="J11" s="18"/>
+      <c r="K11" s="18"/>
+      <c r="L11" s="18"/>
+      <c r="M11" s="28"/>
+      <c r="N11" s="28"/>
+      <c r="O11" s="18"/>
+      <c r="P11" s="18"/>
+      <c r="Q11" s="18"/>
+      <c r="R11" s="18"/>
+      <c r="S11" s="22"/>
+      <c r="T11" s="29"/>
+      <c r="U11" s="22"/>
+      <c r="V11" s="23"/>
+      <c r="W11" s="23"/>
+    </row>
+    <row r="12" spans="1:23" s="22" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="30"/>
+      <c r="B12" s="26"/>
+      <c r="C12" s="27"/>
+      <c r="D12" s="18"/>
+      <c r="E12" s="18"/>
+      <c r="F12" s="18"/>
+      <c r="G12" s="28"/>
+      <c r="H12" s="31"/>
+      <c r="I12" s="32"/>
+      <c r="J12" s="32"/>
+      <c r="K12" s="18"/>
+      <c r="L12" s="33"/>
+      <c r="M12" s="18"/>
+      <c r="N12" s="18"/>
+      <c r="O12" s="18"/>
+      <c r="P12" s="18"/>
+      <c r="Q12" s="18"/>
+    </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="C1:J1"/>
   </mergeCells>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" sqref="L1:L8">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" sqref="L1:L12">
       <formula1>"5000,,7000,,8000"</formula1>
     </dataValidation>
   </dataValidations>
   <hyperlinks>
     <hyperlink ref="D3" r:id="rId1"/>
     <hyperlink ref="D5" r:id="rId2"/>
+    <hyperlink ref="D7" r:id="rId3"/>
+    <hyperlink ref="D9" r:id="rId4"/>
+    <hyperlink ref="D11" r:id="rId5"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId3"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId6"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Changed aftermethod calls. Disabled on test finish
</commit_message>
<xml_diff>
--- a/src/test/resources/testData/Driver.xlsx
+++ b/src/test/resources/testData/Driver.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="41">
   <si>
     <t>Parameteres</t>
   </si>
@@ -102,9 +102,6 @@
   </si>
   <si>
     <t>password</t>
-  </si>
-  <si>
-    <t>rautsumit</t>
   </si>
   <si>
     <t>http://www.newtours.demoaut.com</t>
@@ -869,7 +866,7 @@
         <v>11</v>
       </c>
       <c r="B2" s="19" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C2" s="10" t="s">
         <v>16</v>
@@ -889,7 +886,7 @@
         <v>12</v>
       </c>
       <c r="B3" s="19" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C3" s="10" t="s">
         <v>16</v>
@@ -909,7 +906,7 @@
         <v>24</v>
       </c>
       <c r="B4" s="19" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C4" s="10" t="s">
         <v>16</v>
@@ -981,7 +978,7 @@
         <v>5</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
@@ -1044,7 +1041,7 @@
   <dimension ref="A1:W12"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="84" zoomScaleNormal="84" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+      <selection activeCell="A7" sqref="A7:XFD8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1081,22 +1078,22 @@
         <v>1</v>
       </c>
       <c r="B2" s="21" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C2" s="22" t="s">
         <v>10</v>
       </c>
       <c r="D2" s="22" t="s">
+        <v>31</v>
+      </c>
+      <c r="E2" s="22" t="s">
         <v>32</v>
       </c>
-      <c r="E2" s="22" t="s">
-        <v>33</v>
-      </c>
       <c r="F2" s="22" t="s">
+        <v>35</v>
+      </c>
+      <c r="G2" s="22" t="s">
         <v>36</v>
-      </c>
-      <c r="G2" s="22" t="s">
-        <v>37</v>
       </c>
       <c r="H2" s="22" t="s">
         <v>26</v>
@@ -1121,22 +1118,22 @@
       <c r="A3" s="25"/>
       <c r="B3" s="26"/>
       <c r="C3" s="27" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D3" s="36" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E3" s="18" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="F3" s="18" t="s">
+        <v>37</v>
+      </c>
+      <c r="G3" s="18" t="s">
         <v>38</v>
       </c>
-      <c r="G3" s="18" t="s">
+      <c r="H3" s="18" t="s">
         <v>39</v>
-      </c>
-      <c r="H3" s="18" t="s">
-        <v>40</v>
       </c>
       <c r="I3" s="18"/>
       <c r="J3" s="18"/>
@@ -1177,22 +1174,22 @@
       <c r="A5" s="25"/>
       <c r="B5" s="26"/>
       <c r="C5" s="27" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D5" s="36" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E5" s="18" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="F5" s="18" t="s">
+        <v>37</v>
+      </c>
+      <c r="G5" s="18" t="s">
         <v>38</v>
       </c>
-      <c r="G5" s="18" t="s">
+      <c r="H5" s="18" t="s">
         <v>39</v>
-      </c>
-      <c r="H5" s="18" t="s">
-        <v>40</v>
       </c>
       <c r="I5" s="18"/>
       <c r="J5" s="18"/>
@@ -1229,26 +1226,26 @@
       <c r="P6" s="18"/>
       <c r="Q6" s="18"/>
     </row>
-    <row r="7" spans="1:23" s="24" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:23" s="24" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="25"/>
       <c r="B7" s="26"/>
       <c r="C7" s="27" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D7" s="36" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E7" s="18" t="s">
-        <v>27</v>
+        <v>33</v>
       </c>
       <c r="F7" s="18" t="s">
+        <v>37</v>
+      </c>
+      <c r="G7" s="18" t="s">
         <v>38</v>
       </c>
-      <c r="G7" s="18" t="s">
+      <c r="H7" s="18" t="s">
         <v>39</v>
-      </c>
-      <c r="H7" s="18" t="s">
-        <v>40</v>
       </c>
       <c r="I7" s="18"/>
       <c r="J7" s="18"/>
@@ -1285,26 +1282,26 @@
       <c r="P8" s="18"/>
       <c r="Q8" s="18"/>
     </row>
-    <row r="9" spans="1:23" s="24" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:23" s="24" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="25"/>
       <c r="B9" s="26"/>
       <c r="C9" s="27" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D9" s="36" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E9" s="18" t="s">
-        <v>27</v>
+        <v>33</v>
       </c>
       <c r="F9" s="18" t="s">
+        <v>37</v>
+      </c>
+      <c r="G9" s="18" t="s">
         <v>38</v>
       </c>
-      <c r="G9" s="18" t="s">
+      <c r="H9" s="18" t="s">
         <v>39</v>
-      </c>
-      <c r="H9" s="18" t="s">
-        <v>40</v>
       </c>
       <c r="I9" s="18"/>
       <c r="J9" s="18"/>
@@ -1345,22 +1342,22 @@
       <c r="A11" s="25"/>
       <c r="B11" s="26"/>
       <c r="C11" s="27" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D11" s="36" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E11" s="18" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="F11" s="18" t="s">
+        <v>37</v>
+      </c>
+      <c r="G11" s="18" t="s">
         <v>38</v>
       </c>
-      <c r="G11" s="18" t="s">
+      <c r="H11" s="18" t="s">
         <v>39</v>
-      </c>
-      <c r="H11" s="18" t="s">
-        <v>40</v>
       </c>
       <c r="I11" s="18"/>
       <c r="J11" s="18"/>

</xml_diff>